<commit_message>
- finished extraction from `10.1016/j.ijrmhm.2024.106681`
</commit_message>
<xml_diff>
--- a/DuctilitySearch_Feb24.xlsx
+++ b/DuctilitySearch_Feb24.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="139">
   <si>
     <t>Metadata</t>
   </si>
@@ -480,6 +480,48 @@
   </si>
   <si>
     <t>F8</t>
+  </si>
+  <si>
+    <t>estimated ultimate compressive strength</t>
+  </si>
+  <si>
+    <t>stopped at 50% strain</t>
+  </si>
+  <si>
+    <t>1748e6</t>
+  </si>
+  <si>
+    <t>1853e6</t>
+  </si>
+  <si>
+    <t>2027e6</t>
+  </si>
+  <si>
+    <t>2166e6</t>
+  </si>
+  <si>
+    <t>2376e6</t>
+  </si>
+  <si>
+    <t>2434e6</t>
+  </si>
+  <si>
+    <t>354e6</t>
+  </si>
+  <si>
+    <t>536e6</t>
+  </si>
+  <si>
+    <t>629e6</t>
+  </si>
+  <si>
+    <t>691e6</t>
+  </si>
+  <si>
+    <t>836e6</t>
+  </si>
+  <si>
+    <t>935e6</t>
   </si>
 </sst>
 </file>
@@ -4971,19 +5013,41 @@
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18">
       <c r="A75" s="50"/>
-      <c r="B75" s="85"/>
-      <c r="C75" s="82"/>
-      <c r="D75" s="82"/>
+      <c r="B75" s="85" t="s">
+        <v>110</v>
+      </c>
+      <c r="C75" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="D75" s="82" t="s">
+        <v>66</v>
+      </c>
       <c r="E75" s="85"/>
-      <c r="F75" s="82"/>
-      <c r="G75" s="82"/>
-      <c r="H75" s="82"/>
-      <c r="I75" s="4"/>
-      <c r="J75" s="5"/>
+      <c r="F75" s="82" t="s">
+        <v>125</v>
+      </c>
+      <c r="G75" s="82" t="s">
+        <v>29</v>
+      </c>
+      <c r="H75" s="82" t="s">
+        <v>126</v>
+      </c>
+      <c r="I75" s="4">
+        <v>298</v>
+      </c>
+      <c r="J75" s="5" t="s">
+        <v>127</v>
+      </c>
       <c r="K75" s="5"/>
-      <c r="L75" s="85"/>
-      <c r="M75" s="85"/>
-      <c r="N75" s="85"/>
+      <c r="L75" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="M75" s="85" t="s">
+        <v>124</v>
+      </c>
+      <c r="N75" s="85" t="s">
+        <v>111</v>
+      </c>
       <c r="O75" s="2"/>
       <c r="P75" s="7"/>
       <c r="Q75" s="2"/>
@@ -4993,19 +5057,41 @@
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18">
       <c r="A76" s="50"/>
-      <c r="B76" s="85"/>
-      <c r="C76" s="82"/>
-      <c r="D76" s="82"/>
+      <c r="B76" s="85" t="s">
+        <v>112</v>
+      </c>
+      <c r="C76" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="D76" s="82" t="s">
+        <v>66</v>
+      </c>
       <c r="E76" s="85"/>
-      <c r="F76" s="82"/>
-      <c r="G76" s="82"/>
-      <c r="H76" s="82"/>
-      <c r="I76" s="4"/>
-      <c r="J76" s="5"/>
+      <c r="F76" s="82" t="s">
+        <v>125</v>
+      </c>
+      <c r="G76" s="82" t="s">
+        <v>29</v>
+      </c>
+      <c r="H76" s="82" t="s">
+        <v>126</v>
+      </c>
+      <c r="I76" s="4">
+        <v>298</v>
+      </c>
+      <c r="J76" s="5" t="s">
+        <v>128</v>
+      </c>
       <c r="K76" s="5"/>
-      <c r="L76" s="85"/>
-      <c r="M76" s="85"/>
-      <c r="N76" s="85"/>
+      <c r="L76" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="M76" s="85" t="s">
+        <v>124</v>
+      </c>
+      <c r="N76" s="85" t="s">
+        <v>111</v>
+      </c>
       <c r="O76" s="2"/>
       <c r="P76" s="7"/>
       <c r="Q76" s="2"/>
@@ -5015,19 +5101,41 @@
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18">
       <c r="A77" s="50"/>
-      <c r="B77" s="85"/>
-      <c r="C77" s="82"/>
-      <c r="D77" s="82"/>
+      <c r="B77" s="85" t="s">
+        <v>113</v>
+      </c>
+      <c r="C77" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="D77" s="82" t="s">
+        <v>66</v>
+      </c>
       <c r="E77" s="85"/>
-      <c r="F77" s="82"/>
-      <c r="G77" s="82"/>
-      <c r="H77" s="82"/>
-      <c r="I77" s="4"/>
-      <c r="J77" s="5"/>
+      <c r="F77" s="82" t="s">
+        <v>125</v>
+      </c>
+      <c r="G77" s="82" t="s">
+        <v>29</v>
+      </c>
+      <c r="H77" s="82" t="s">
+        <v>126</v>
+      </c>
+      <c r="I77" s="4">
+        <v>298</v>
+      </c>
+      <c r="J77" s="5" t="s">
+        <v>129</v>
+      </c>
       <c r="K77" s="5"/>
-      <c r="L77" s="85"/>
-      <c r="M77" s="85"/>
-      <c r="N77" s="85"/>
+      <c r="L77" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="M77" s="85" t="s">
+        <v>124</v>
+      </c>
+      <c r="N77" s="85" t="s">
+        <v>111</v>
+      </c>
       <c r="O77" s="2"/>
       <c r="P77" s="7"/>
       <c r="Q77" s="2"/>
@@ -5037,19 +5145,41 @@
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18">
       <c r="A78" s="50"/>
-      <c r="B78" s="85"/>
-      <c r="C78" s="82"/>
-      <c r="D78" s="82"/>
+      <c r="B78" s="85" t="s">
+        <v>114</v>
+      </c>
+      <c r="C78" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="D78" s="82" t="s">
+        <v>66</v>
+      </c>
       <c r="E78" s="85"/>
-      <c r="F78" s="82"/>
-      <c r="G78" s="82"/>
-      <c r="H78" s="82"/>
-      <c r="I78" s="4"/>
-      <c r="J78" s="5"/>
+      <c r="F78" s="82" t="s">
+        <v>125</v>
+      </c>
+      <c r="G78" s="82" t="s">
+        <v>29</v>
+      </c>
+      <c r="H78" s="82" t="s">
+        <v>126</v>
+      </c>
+      <c r="I78" s="4">
+        <v>298</v>
+      </c>
+      <c r="J78" s="5" t="s">
+        <v>130</v>
+      </c>
       <c r="K78" s="5"/>
-      <c r="L78" s="85"/>
-      <c r="M78" s="85"/>
-      <c r="N78" s="85"/>
+      <c r="L78" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="M78" s="85" t="s">
+        <v>124</v>
+      </c>
+      <c r="N78" s="85" t="s">
+        <v>111</v>
+      </c>
       <c r="O78" s="2"/>
       <c r="P78" s="7"/>
       <c r="Q78" s="2"/>
@@ -5059,19 +5189,41 @@
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18">
       <c r="A79" s="50"/>
-      <c r="B79" s="85"/>
-      <c r="C79" s="82"/>
-      <c r="D79" s="82"/>
+      <c r="B79" s="85" t="s">
+        <v>115</v>
+      </c>
+      <c r="C79" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="D79" s="82" t="s">
+        <v>66</v>
+      </c>
       <c r="E79" s="85"/>
-      <c r="F79" s="82"/>
-      <c r="G79" s="82"/>
-      <c r="H79" s="82"/>
-      <c r="I79" s="4"/>
-      <c r="J79" s="5"/>
+      <c r="F79" s="82" t="s">
+        <v>125</v>
+      </c>
+      <c r="G79" s="82" t="s">
+        <v>29</v>
+      </c>
+      <c r="H79" s="82" t="s">
+        <v>126</v>
+      </c>
+      <c r="I79" s="4">
+        <v>298</v>
+      </c>
+      <c r="J79" s="5" t="s">
+        <v>131</v>
+      </c>
       <c r="K79" s="5"/>
-      <c r="L79" s="85"/>
-      <c r="M79" s="85"/>
-      <c r="N79" s="85"/>
+      <c r="L79" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="M79" s="85" t="s">
+        <v>124</v>
+      </c>
+      <c r="N79" s="85" t="s">
+        <v>111</v>
+      </c>
       <c r="O79" s="2"/>
       <c r="P79" s="7"/>
       <c r="Q79" s="2"/>
@@ -5081,19 +5233,41 @@
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18">
       <c r="A80" s="50"/>
-      <c r="B80" s="85"/>
-      <c r="C80" s="82"/>
-      <c r="D80" s="82"/>
+      <c r="B80" s="85" t="s">
+        <v>116</v>
+      </c>
+      <c r="C80" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="D80" s="82" t="s">
+        <v>66</v>
+      </c>
       <c r="E80" s="85"/>
-      <c r="F80" s="82"/>
-      <c r="G80" s="82"/>
-      <c r="H80" s="82"/>
-      <c r="I80" s="4"/>
-      <c r="J80" s="5"/>
+      <c r="F80" s="82" t="s">
+        <v>125</v>
+      </c>
+      <c r="G80" s="82" t="s">
+        <v>29</v>
+      </c>
+      <c r="H80" s="82" t="s">
+        <v>126</v>
+      </c>
+      <c r="I80" s="4">
+        <v>298</v>
+      </c>
+      <c r="J80" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="K80" s="5"/>
-      <c r="L80" s="85"/>
-      <c r="M80" s="85"/>
-      <c r="N80" s="85"/>
+      <c r="L80" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="M80" s="85" t="s">
+        <v>124</v>
+      </c>
+      <c r="N80" s="85" t="s">
+        <v>111</v>
+      </c>
       <c r="O80" s="2"/>
       <c r="P80" s="7"/>
       <c r="Q80" s="2"/>
@@ -5103,19 +5277,39 @@
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18">
       <c r="A81" s="50"/>
-      <c r="B81" s="85"/>
-      <c r="C81" s="82"/>
-      <c r="D81" s="82"/>
+      <c r="B81" s="85" t="s">
+        <v>110</v>
+      </c>
+      <c r="C81" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="D81" s="82" t="s">
+        <v>66</v>
+      </c>
       <c r="E81" s="85"/>
-      <c r="F81" s="82"/>
-      <c r="G81" s="82"/>
+      <c r="F81" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="G81" s="82" t="s">
+        <v>29</v>
+      </c>
       <c r="H81" s="82"/>
-      <c r="I81" s="4"/>
-      <c r="J81" s="5"/>
+      <c r="I81" s="4">
+        <v>298</v>
+      </c>
+      <c r="J81" s="5" t="s">
+        <v>133</v>
+      </c>
       <c r="K81" s="5"/>
-      <c r="L81" s="85"/>
-      <c r="M81" s="85"/>
-      <c r="N81" s="85"/>
+      <c r="L81" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="M81" s="85" t="s">
+        <v>124</v>
+      </c>
+      <c r="N81" s="85" t="s">
+        <v>111</v>
+      </c>
       <c r="O81" s="2"/>
       <c r="P81" s="7"/>
       <c r="Q81" s="2"/>
@@ -5125,19 +5319,39 @@
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18">
       <c r="A82" s="50"/>
-      <c r="B82" s="85"/>
-      <c r="C82" s="82"/>
-      <c r="D82" s="82"/>
+      <c r="B82" s="85" t="s">
+        <v>112</v>
+      </c>
+      <c r="C82" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="D82" s="82" t="s">
+        <v>66</v>
+      </c>
       <c r="E82" s="85"/>
-      <c r="F82" s="82"/>
-      <c r="G82" s="82"/>
+      <c r="F82" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="G82" s="82" t="s">
+        <v>29</v>
+      </c>
       <c r="H82" s="82"/>
-      <c r="I82" s="4"/>
-      <c r="J82" s="5"/>
+      <c r="I82" s="4">
+        <v>298</v>
+      </c>
+      <c r="J82" s="5" t="s">
+        <v>134</v>
+      </c>
       <c r="K82" s="5"/>
-      <c r="L82" s="85"/>
-      <c r="M82" s="85"/>
-      <c r="N82" s="85"/>
+      <c r="L82" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="M82" s="85" t="s">
+        <v>124</v>
+      </c>
+      <c r="N82" s="85" t="s">
+        <v>111</v>
+      </c>
       <c r="O82" s="2"/>
       <c r="P82" s="7"/>
       <c r="Q82" s="2"/>
@@ -5147,19 +5361,39 @@
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18">
       <c r="A83" s="50"/>
-      <c r="B83" s="85"/>
-      <c r="C83" s="82"/>
-      <c r="D83" s="82"/>
+      <c r="B83" s="85" t="s">
+        <v>113</v>
+      </c>
+      <c r="C83" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="D83" s="82" t="s">
+        <v>66</v>
+      </c>
       <c r="E83" s="85"/>
-      <c r="F83" s="82"/>
-      <c r="G83" s="82"/>
+      <c r="F83" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="G83" s="82" t="s">
+        <v>29</v>
+      </c>
       <c r="H83" s="82"/>
-      <c r="I83" s="4"/>
-      <c r="J83" s="5"/>
+      <c r="I83" s="4">
+        <v>298</v>
+      </c>
+      <c r="J83" s="5" t="s">
+        <v>135</v>
+      </c>
       <c r="K83" s="5"/>
-      <c r="L83" s="85"/>
-      <c r="M83" s="85"/>
-      <c r="N83" s="85"/>
+      <c r="L83" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="M83" s="85" t="s">
+        <v>124</v>
+      </c>
+      <c r="N83" s="85" t="s">
+        <v>111</v>
+      </c>
       <c r="O83" s="2"/>
       <c r="P83" s="7"/>
       <c r="Q83" s="2"/>
@@ -5169,19 +5403,39 @@
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18">
       <c r="A84" s="50"/>
-      <c r="B84" s="85"/>
-      <c r="C84" s="82"/>
-      <c r="D84" s="82"/>
+      <c r="B84" s="85" t="s">
+        <v>114</v>
+      </c>
+      <c r="C84" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="D84" s="82" t="s">
+        <v>66</v>
+      </c>
       <c r="E84" s="85"/>
-      <c r="F84" s="82"/>
-      <c r="G84" s="82"/>
+      <c r="F84" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="G84" s="82" t="s">
+        <v>29</v>
+      </c>
       <c r="H84" s="82"/>
-      <c r="I84" s="4"/>
-      <c r="J84" s="5"/>
+      <c r="I84" s="4">
+        <v>298</v>
+      </c>
+      <c r="J84" s="5" t="s">
+        <v>136</v>
+      </c>
       <c r="K84" s="5"/>
-      <c r="L84" s="85"/>
-      <c r="M84" s="85"/>
-      <c r="N84" s="85"/>
+      <c r="L84" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="M84" s="85" t="s">
+        <v>124</v>
+      </c>
+      <c r="N84" s="85" t="s">
+        <v>111</v>
+      </c>
       <c r="O84" s="2"/>
       <c r="P84" s="7"/>
       <c r="Q84" s="2"/>
@@ -5191,19 +5445,39 @@
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18">
       <c r="A85" s="50"/>
-      <c r="B85" s="85"/>
-      <c r="C85" s="82"/>
-      <c r="D85" s="82"/>
+      <c r="B85" s="85" t="s">
+        <v>115</v>
+      </c>
+      <c r="C85" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="D85" s="82" t="s">
+        <v>66</v>
+      </c>
       <c r="E85" s="85"/>
-      <c r="F85" s="82"/>
-      <c r="G85" s="82"/>
+      <c r="F85" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="G85" s="82" t="s">
+        <v>29</v>
+      </c>
       <c r="H85" s="82"/>
-      <c r="I85" s="4"/>
-      <c r="J85" s="5"/>
+      <c r="I85" s="4">
+        <v>298</v>
+      </c>
+      <c r="J85" s="5" t="s">
+        <v>137</v>
+      </c>
       <c r="K85" s="5"/>
-      <c r="L85" s="85"/>
-      <c r="M85" s="85"/>
-      <c r="N85" s="85"/>
+      <c r="L85" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="M85" s="85" t="s">
+        <v>124</v>
+      </c>
+      <c r="N85" s="85" t="s">
+        <v>111</v>
+      </c>
       <c r="O85" s="2"/>
       <c r="P85" s="7"/>
       <c r="Q85" s="2"/>
@@ -5213,19 +5487,39 @@
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18">
       <c r="A86" s="50"/>
-      <c r="B86" s="85"/>
-      <c r="C86" s="82"/>
-      <c r="D86" s="82"/>
+      <c r="B86" s="85" t="s">
+        <v>116</v>
+      </c>
+      <c r="C86" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="D86" s="82" t="s">
+        <v>66</v>
+      </c>
       <c r="E86" s="85"/>
-      <c r="F86" s="82"/>
-      <c r="G86" s="82"/>
+      <c r="F86" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="G86" s="82" t="s">
+        <v>29</v>
+      </c>
       <c r="H86" s="82"/>
-      <c r="I86" s="4"/>
-      <c r="J86" s="5"/>
+      <c r="I86" s="4">
+        <v>298</v>
+      </c>
+      <c r="J86" s="5" t="s">
+        <v>138</v>
+      </c>
       <c r="K86" s="5"/>
-      <c r="L86" s="85"/>
-      <c r="M86" s="85"/>
-      <c r="N86" s="85"/>
+      <c r="L86" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="M86" s="85" t="s">
+        <v>124</v>
+      </c>
+      <c r="N86" s="85" t="s">
+        <v>111</v>
+      </c>
       <c r="O86" s="2"/>
       <c r="P86" s="7"/>
       <c r="Q86" s="2"/>

</xml_diff>

<commit_message>
- extracted data from `10.1038/s41563-024-01871-7`
</commit_message>
<xml_diff>
--- a/DuctilitySearch_Feb24.xlsx
+++ b/DuctilitySearch_Feb24.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="238">
   <si>
     <t>Metadata</t>
   </si>
@@ -764,9 +764,6 @@
     <t>10.1016/j.jallcom.2024.174459</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Ti Zr Nb Mo Ta0.9</t>
   </si>
   <si>
@@ -780,6 +777,48 @@
   </si>
   <si>
     <t>strain rate 0.5e-3</t>
+  </si>
+  <si>
+    <t>V33 Co34 Ni33</t>
+  </si>
+  <si>
+    <t>FCC+L12+HCP</t>
+  </si>
+  <si>
+    <t>VAM+HF+H+CR+RX</t>
+  </si>
+  <si>
+    <t>Lamellar phases in FCC grains; ultrafine grain 0.43um; hot forged at 1,423 K; homogenization in a vacuum at 1,373 K for 2 h; cold rolling for 90% reduction; recrystallization at 1,173 K for 150s</t>
+  </si>
+  <si>
+    <t>tensile yield strength</t>
+  </si>
+  <si>
+    <t>2.08e9</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>strain rate 0.5e-3; liquid nitrogen</t>
+  </si>
+  <si>
+    <t>2.25e9</t>
+  </si>
+  <si>
+    <t>strain rate 0.5e-3; liquid helium</t>
+  </si>
+  <si>
+    <t>2.3e9</t>
+  </si>
+  <si>
+    <t>ultimate tensile strength</t>
+  </si>
+  <si>
+    <t>2.04e9</t>
+  </si>
+  <si>
+    <t>2.35e9</t>
   </si>
 </sst>
 </file>
@@ -1366,7 +1405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="91">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1619,9 +1658,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1949,26 +1985,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="86" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="87" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="88" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="88" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="87" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="88" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="88" width="19.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="88" width="21.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="89" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="90" width="25.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="90" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="91" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="91" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="91" width="34.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="87" width="39.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="86" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="87" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="87" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="87" width="17.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="87" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="85" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="86" width="31.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="87" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="87" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="86" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="87" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="87" width="19.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="87" width="21.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="88" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="89" width="25.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="89" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="90" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="90" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="90" width="34.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="86" width="39.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="85" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="86" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="86" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="86" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="86" width="17.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
@@ -8311,19 +8347,19 @@
       <c r="A141" s="49">
         <v>8</v>
       </c>
-      <c r="B141" s="7" t="s">
+      <c r="B141" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C141" s="80" t="s">
+      <c r="C141" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D141" s="80" t="s">
+      <c r="D141" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E141" s="7" t="s">
+      <c r="E141" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="F141" s="80" t="s">
+      <c r="F141" s="3" t="s">
         <v>82</v>
       </c>
       <c r="G141" s="3" t="s">
@@ -8339,19 +8375,17 @@
       <c r="K141" s="5">
         <v>0.07</v>
       </c>
-      <c r="L141" s="7" t="s">
+      <c r="L141" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="M141" s="7" t="s">
+      <c r="M141" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="N141" s="7" t="s">
+      <c r="N141" s="6" t="s">
         <v>218</v>
       </c>
       <c r="O141" s="2"/>
-      <c r="P141" s="85" t="s">
-        <v>219</v>
-      </c>
+      <c r="P141" s="7"/>
       <c r="Q141" s="2"/>
       <c r="R141" s="2"/>
       <c r="S141" s="2"/>
@@ -8361,19 +8395,19 @@
       <c r="A142" s="49">
         <v>8</v>
       </c>
-      <c r="B142" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="C142" s="80" t="s">
+      <c r="B142" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C142" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D142" s="80" t="s">
+      <c r="D142" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E142" s="7" t="s">
+      <c r="E142" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="F142" s="80" t="s">
+      <c r="F142" s="3" t="s">
         <v>82</v>
       </c>
       <c r="G142" s="3" t="s">
@@ -8389,19 +8423,17 @@
       <c r="K142" s="5">
         <v>0.05</v>
       </c>
-      <c r="L142" s="7" t="s">
+      <c r="L142" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="M142" s="7" t="s">
+      <c r="M142" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="N142" s="7" t="s">
+      <c r="N142" s="6" t="s">
         <v>218</v>
       </c>
       <c r="O142" s="2"/>
-      <c r="P142" s="85" t="s">
-        <v>219</v>
-      </c>
+      <c r="P142" s="7"/>
       <c r="Q142" s="2"/>
       <c r="R142" s="2"/>
       <c r="S142" s="2"/>
@@ -8411,19 +8443,19 @@
       <c r="A143" s="49">
         <v>8</v>
       </c>
-      <c r="B143" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="C143" s="80" t="s">
+      <c r="B143" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C143" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D143" s="80" t="s">
+      <c r="D143" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E143" s="7" t="s">
+      <c r="E143" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="F143" s="80" t="s">
+      <c r="F143" s="3" t="s">
         <v>82</v>
       </c>
       <c r="G143" s="3" t="s">
@@ -8439,19 +8471,17 @@
       <c r="K143" s="5">
         <v>0.04</v>
       </c>
-      <c r="L143" s="7" t="s">
+      <c r="L143" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="M143" s="7" t="s">
+      <c r="M143" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="N143" s="7" t="s">
+      <c r="N143" s="6" t="s">
         <v>218</v>
       </c>
       <c r="O143" s="2"/>
-      <c r="P143" s="85" t="s">
-        <v>219</v>
-      </c>
+      <c r="P143" s="7"/>
       <c r="Q143" s="2"/>
       <c r="R143" s="2"/>
       <c r="S143" s="2"/>
@@ -8461,19 +8491,19 @@
       <c r="A144" s="49">
         <v>8</v>
       </c>
-      <c r="B144" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="C144" s="80" t="s">
+      <c r="B144" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="C144" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D144" s="80" t="s">
+      <c r="D144" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E144" s="7" t="s">
+      <c r="E144" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="F144" s="80" t="s">
+      <c r="F144" s="3" t="s">
         <v>82</v>
       </c>
       <c r="G144" s="3" t="s">
@@ -8489,19 +8519,17 @@
       <c r="K144" s="5">
         <v>0.02</v>
       </c>
-      <c r="L144" s="7" t="s">
+      <c r="L144" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="M144" s="7" t="s">
+      <c r="M144" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="N144" s="7" t="s">
+      <c r="N144" s="6" t="s">
         <v>218</v>
       </c>
       <c r="O144" s="2"/>
-      <c r="P144" s="85" t="s">
-        <v>219</v>
-      </c>
+      <c r="P144" s="7"/>
       <c r="Q144" s="2"/>
       <c r="R144" s="2"/>
       <c r="S144" s="2"/>
@@ -8511,19 +8539,19 @@
       <c r="A145" s="49">
         <v>8</v>
       </c>
-      <c r="B145" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="C145" s="80" t="s">
+      <c r="B145" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C145" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D145" s="80" t="s">
+      <c r="D145" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E145" s="7" t="s">
+      <c r="E145" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="F145" s="80" t="s">
+      <c r="F145" s="3" t="s">
         <v>82</v>
       </c>
       <c r="G145" s="3" t="s">
@@ -8539,19 +8567,17 @@
       <c r="K145" s="5">
         <v>0.06</v>
       </c>
-      <c r="L145" s="7" t="s">
+      <c r="L145" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="M145" s="7" t="s">
+      <c r="M145" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="N145" s="7" t="s">
+      <c r="N145" s="6" t="s">
         <v>218</v>
       </c>
       <c r="O145" s="2"/>
-      <c r="P145" s="85" t="s">
-        <v>219</v>
-      </c>
+      <c r="P145" s="7"/>
       <c r="Q145" s="2"/>
       <c r="R145" s="2"/>
       <c r="S145" s="2"/>
@@ -8561,26 +8587,26 @@
       <c r="A146" s="49">
         <v>8</v>
       </c>
-      <c r="B146" s="7" t="s">
+      <c r="B146" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C146" s="80" t="s">
+      <c r="C146" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D146" s="80" t="s">
+      <c r="D146" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E146" s="7" t="s">
+      <c r="E146" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="F146" s="80" t="s">
+      <c r="F146" s="3" t="s">
         <v>142</v>
       </c>
       <c r="G146" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H146" s="80" t="s">
-        <v>224</v>
+      <c r="H146" s="3" t="s">
+        <v>223</v>
       </c>
       <c r="I146" s="4">
         <v>298</v>
@@ -8591,13 +8617,13 @@
       <c r="K146" s="5">
         <v>38000000</v>
       </c>
-      <c r="L146" s="7" t="s">
+      <c r="L146" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M146" s="7" t="s">
+      <c r="M146" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N146" s="7" t="s">
+      <c r="N146" s="6" t="s">
         <v>218</v>
       </c>
       <c r="O146" s="2"/>
@@ -8611,26 +8637,26 @@
       <c r="A147" s="49">
         <v>8</v>
       </c>
-      <c r="B147" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="C147" s="80" t="s">
+      <c r="B147" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C147" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D147" s="80" t="s">
+      <c r="D147" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E147" s="7" t="s">
+      <c r="E147" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="F147" s="80" t="s">
+      <c r="F147" s="3" t="s">
         <v>142</v>
       </c>
       <c r="G147" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H147" s="80" t="s">
-        <v>224</v>
+      <c r="H147" s="3" t="s">
+        <v>223</v>
       </c>
       <c r="I147" s="4">
         <v>298</v>
@@ -8641,13 +8667,13 @@
       <c r="K147" s="5">
         <v>25000000</v>
       </c>
-      <c r="L147" s="7" t="s">
+      <c r="L147" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M147" s="7" t="s">
+      <c r="M147" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N147" s="7" t="s">
+      <c r="N147" s="6" t="s">
         <v>218</v>
       </c>
       <c r="O147" s="2"/>
@@ -8661,26 +8687,26 @@
       <c r="A148" s="49">
         <v>8</v>
       </c>
-      <c r="B148" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="C148" s="80" t="s">
+      <c r="B148" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C148" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D148" s="80" t="s">
+      <c r="D148" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E148" s="7" t="s">
+      <c r="E148" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="F148" s="80" t="s">
+      <c r="F148" s="3" t="s">
         <v>142</v>
       </c>
       <c r="G148" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H148" s="80" t="s">
-        <v>224</v>
+      <c r="H148" s="3" t="s">
+        <v>223</v>
       </c>
       <c r="I148" s="4">
         <v>298</v>
@@ -8691,13 +8717,13 @@
       <c r="K148" s="5">
         <v>17000000</v>
       </c>
-      <c r="L148" s="7" t="s">
+      <c r="L148" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M148" s="7" t="s">
+      <c r="M148" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N148" s="7" t="s">
+      <c r="N148" s="6" t="s">
         <v>218</v>
       </c>
       <c r="O148" s="2"/>
@@ -8711,26 +8737,26 @@
       <c r="A149" s="49">
         <v>8</v>
       </c>
-      <c r="B149" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="C149" s="80" t="s">
+      <c r="B149" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="C149" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D149" s="80" t="s">
+      <c r="D149" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E149" s="7" t="s">
+      <c r="E149" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="F149" s="80" t="s">
+      <c r="F149" s="3" t="s">
         <v>142</v>
       </c>
       <c r="G149" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H149" s="80" t="s">
-        <v>224</v>
+      <c r="H149" s="3" t="s">
+        <v>223</v>
       </c>
       <c r="I149" s="4">
         <v>298</v>
@@ -8741,13 +8767,13 @@
       <c r="K149" s="5">
         <v>23000000</v>
       </c>
-      <c r="L149" s="7" t="s">
+      <c r="L149" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M149" s="7" t="s">
+      <c r="M149" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N149" s="7" t="s">
+      <c r="N149" s="6" t="s">
         <v>218</v>
       </c>
       <c r="O149" s="2"/>
@@ -8761,26 +8787,26 @@
       <c r="A150" s="49">
         <v>8</v>
       </c>
-      <c r="B150" s="7" t="s">
+      <c r="B150" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E150" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F150" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G150" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H150" s="3" t="s">
         <v>223</v>
-      </c>
-      <c r="C150" s="80" t="s">
-        <v>215</v>
-      </c>
-      <c r="D150" s="80" t="s">
-        <v>216</v>
-      </c>
-      <c r="E150" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="F150" s="80" t="s">
-        <v>142</v>
-      </c>
-      <c r="G150" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H150" s="80" t="s">
-        <v>224</v>
       </c>
       <c r="I150" s="4">
         <v>298</v>
@@ -8791,13 +8817,13 @@
       <c r="K150" s="5">
         <v>16000000</v>
       </c>
-      <c r="L150" s="7" t="s">
+      <c r="L150" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M150" s="7" t="s">
+      <c r="M150" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N150" s="7" t="s">
+      <c r="N150" s="6" t="s">
         <v>218</v>
       </c>
       <c r="O150" s="2"/>
@@ -8811,26 +8837,26 @@
       <c r="A151" s="49">
         <v>8</v>
       </c>
-      <c r="B151" s="7" t="s">
+      <c r="B151" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C151" s="80" t="s">
+      <c r="C151" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D151" s="80" t="s">
+      <c r="D151" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E151" s="7" t="s">
+      <c r="E151" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="F151" s="80" t="s">
+      <c r="F151" s="3" t="s">
         <v>107</v>
       </c>
       <c r="G151" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H151" s="80" t="s">
-        <v>224</v>
+      <c r="H151" s="3" t="s">
+        <v>223</v>
       </c>
       <c r="I151" s="4">
         <v>298</v>
@@ -8841,13 +8867,13 @@
       <c r="K151" s="5">
         <v>1.2</v>
       </c>
-      <c r="L151" s="7" t="s">
+      <c r="L151" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M151" s="7" t="s">
+      <c r="M151" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N151" s="7" t="s">
+      <c r="N151" s="6" t="s">
         <v>218</v>
       </c>
       <c r="O151" s="2"/>
@@ -8861,26 +8887,26 @@
       <c r="A152" s="49">
         <v>8</v>
       </c>
-      <c r="B152" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="C152" s="80" t="s">
+      <c r="B152" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C152" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D152" s="80" t="s">
+      <c r="D152" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E152" s="7" t="s">
+      <c r="E152" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="F152" s="80" t="s">
+      <c r="F152" s="3" t="s">
         <v>107</v>
       </c>
       <c r="G152" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H152" s="80" t="s">
-        <v>224</v>
+      <c r="H152" s="3" t="s">
+        <v>223</v>
       </c>
       <c r="I152" s="4">
         <v>298</v>
@@ -8891,13 +8917,13 @@
       <c r="K152" s="5">
         <v>2.7</v>
       </c>
-      <c r="L152" s="7" t="s">
+      <c r="L152" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M152" s="7" t="s">
+      <c r="M152" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N152" s="7" t="s">
+      <c r="N152" s="6" t="s">
         <v>218</v>
       </c>
       <c r="O152" s="2"/>
@@ -8911,26 +8937,26 @@
       <c r="A153" s="49">
         <v>8</v>
       </c>
-      <c r="B153" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="C153" s="80" t="s">
+      <c r="B153" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C153" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D153" s="80" t="s">
+      <c r="D153" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E153" s="7" t="s">
+      <c r="E153" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="F153" s="80" t="s">
+      <c r="F153" s="3" t="s">
         <v>107</v>
       </c>
       <c r="G153" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H153" s="80" t="s">
-        <v>224</v>
+      <c r="H153" s="3" t="s">
+        <v>223</v>
       </c>
       <c r="I153" s="4">
         <v>298</v>
@@ -8941,13 +8967,13 @@
       <c r="K153" s="5">
         <v>1.5</v>
       </c>
-      <c r="L153" s="7" t="s">
+      <c r="L153" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M153" s="7" t="s">
+      <c r="M153" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N153" s="7" t="s">
+      <c r="N153" s="6" t="s">
         <v>218</v>
       </c>
       <c r="O153" s="2"/>
@@ -8961,26 +8987,26 @@
       <c r="A154" s="49">
         <v>8</v>
       </c>
-      <c r="B154" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="C154" s="80" t="s">
+      <c r="B154" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="C154" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D154" s="80" t="s">
+      <c r="D154" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E154" s="7" t="s">
+      <c r="E154" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="F154" s="80" t="s">
+      <c r="F154" s="3" t="s">
         <v>107</v>
       </c>
       <c r="G154" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H154" s="80" t="s">
-        <v>224</v>
+      <c r="H154" s="3" t="s">
+        <v>223</v>
       </c>
       <c r="I154" s="4">
         <v>298</v>
@@ -8991,13 +9017,13 @@
       <c r="K154" s="5">
         <v>4.1</v>
       </c>
-      <c r="L154" s="7" t="s">
+      <c r="L154" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M154" s="7" t="s">
+      <c r="M154" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N154" s="7" t="s">
+      <c r="N154" s="6" t="s">
         <v>218</v>
       </c>
       <c r="O154" s="2"/>
@@ -9011,26 +9037,26 @@
       <c r="A155" s="49">
         <v>8</v>
       </c>
-      <c r="B155" s="7" t="s">
+      <c r="B155" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D155" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E155" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F155" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G155" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H155" s="3" t="s">
         <v>223</v>
-      </c>
-      <c r="C155" s="80" t="s">
-        <v>215</v>
-      </c>
-      <c r="D155" s="80" t="s">
-        <v>216</v>
-      </c>
-      <c r="E155" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="F155" s="80" t="s">
-        <v>107</v>
-      </c>
-      <c r="G155" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H155" s="80" t="s">
-        <v>224</v>
       </c>
       <c r="I155" s="4">
         <v>298</v>
@@ -9041,13 +9067,13 @@
       <c r="K155" s="5">
         <v>2.6</v>
       </c>
-      <c r="L155" s="7" t="s">
+      <c r="L155" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M155" s="7" t="s">
+      <c r="M155" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N155" s="7" t="s">
+      <c r="N155" s="6" t="s">
         <v>218</v>
       </c>
       <c r="O155" s="2"/>
@@ -9061,19 +9087,19 @@
       <c r="A156" s="49">
         <v>8</v>
       </c>
-      <c r="B156" s="7" t="s">
+      <c r="B156" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C156" s="80" t="s">
+      <c r="C156" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D156" s="80" t="s">
+      <c r="D156" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E156" s="7" t="s">
+      <c r="E156" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="F156" s="80" t="s">
+      <c r="F156" s="3" t="s">
         <v>108</v>
       </c>
       <c r="G156" s="3" t="s">
@@ -9089,13 +9115,13 @@
       <c r="K156" s="5">
         <v>70610400</v>
       </c>
-      <c r="L156" s="7" t="s">
+      <c r="L156" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M156" s="7" t="s">
+      <c r="M156" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N156" s="7" t="s">
+      <c r="N156" s="6" t="s">
         <v>218</v>
       </c>
       <c r="O156" s="2"/>
@@ -9109,19 +9135,19 @@
       <c r="A157" s="49">
         <v>8</v>
       </c>
-      <c r="B157" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="C157" s="80" t="s">
+      <c r="B157" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C157" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D157" s="80" t="s">
+      <c r="D157" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E157" s="7" t="s">
+      <c r="E157" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="F157" s="80" t="s">
+      <c r="F157" s="3" t="s">
         <v>108</v>
       </c>
       <c r="G157" s="3" t="s">
@@ -9137,13 +9163,13 @@
       <c r="K157" s="5">
         <v>47073600</v>
       </c>
-      <c r="L157" s="7" t="s">
+      <c r="L157" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M157" s="7" t="s">
+      <c r="M157" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N157" s="7" t="s">
+      <c r="N157" s="6" t="s">
         <v>218</v>
       </c>
       <c r="O157" s="2"/>
@@ -9157,19 +9183,19 @@
       <c r="A158" s="49">
         <v>8</v>
       </c>
-      <c r="B158" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="C158" s="80" t="s">
+      <c r="B158" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C158" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D158" s="80" t="s">
+      <c r="D158" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E158" s="7" t="s">
+      <c r="E158" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="F158" s="80" t="s">
+      <c r="F158" s="3" t="s">
         <v>108</v>
       </c>
       <c r="G158" s="3" t="s">
@@ -9185,13 +9211,13 @@
       <c r="K158" s="5">
         <v>103954200</v>
       </c>
-      <c r="L158" s="7" t="s">
+      <c r="L158" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M158" s="7" t="s">
+      <c r="M158" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N158" s="7" t="s">
+      <c r="N158" s="6" t="s">
         <v>218</v>
       </c>
       <c r="O158" s="2"/>
@@ -9205,19 +9231,19 @@
       <c r="A159" s="49">
         <v>8</v>
       </c>
-      <c r="B159" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="C159" s="80" t="s">
+      <c r="B159" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="C159" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D159" s="80" t="s">
+      <c r="D159" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E159" s="7" t="s">
+      <c r="E159" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="F159" s="80" t="s">
+      <c r="F159" s="3" t="s">
         <v>108</v>
       </c>
       <c r="G159" s="3" t="s">
@@ -9233,13 +9259,13 @@
       <c r="K159" s="5">
         <v>80417400</v>
       </c>
-      <c r="L159" s="7" t="s">
+      <c r="L159" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M159" s="7" t="s">
+      <c r="M159" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N159" s="7" t="s">
+      <c r="N159" s="6" t="s">
         <v>218</v>
       </c>
       <c r="O159" s="2"/>
@@ -9253,19 +9279,19 @@
       <c r="A160" s="49">
         <v>8</v>
       </c>
-      <c r="B160" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="C160" s="80" t="s">
+      <c r="B160" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C160" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D160" s="80" t="s">
+      <c r="D160" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E160" s="7" t="s">
+      <c r="E160" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="F160" s="80" t="s">
+      <c r="F160" s="3" t="s">
         <v>108</v>
       </c>
       <c r="G160" s="3" t="s">
@@ -9281,13 +9307,13 @@
       <c r="K160" s="5">
         <v>46092900</v>
       </c>
-      <c r="L160" s="7" t="s">
+      <c r="L160" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M160" s="7" t="s">
+      <c r="M160" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N160" s="7" t="s">
+      <c r="N160" s="6" t="s">
         <v>218</v>
       </c>
       <c r="O160" s="2"/>
@@ -9298,19 +9324,43 @@
       <c r="T160" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18">
-      <c r="A161" s="49"/>
-      <c r="B161" s="7"/>
-      <c r="C161" s="80"/>
-      <c r="D161" s="80"/>
-      <c r="E161" s="7"/>
-      <c r="F161" s="80"/>
-      <c r="G161" s="80"/>
-      <c r="H161" s="80"/>
-      <c r="I161" s="4"/>
-      <c r="J161" s="5"/>
+      <c r="A161" s="49">
+        <v>9</v>
+      </c>
+      <c r="B161" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C161" s="80" t="s">
+        <v>225</v>
+      </c>
+      <c r="D161" s="80" t="s">
+        <v>226</v>
+      </c>
+      <c r="E161" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="F161" s="80" t="s">
+        <v>228</v>
+      </c>
+      <c r="G161" s="80" t="s">
+        <v>29</v>
+      </c>
+      <c r="H161" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="I161" s="4">
+        <v>298</v>
+      </c>
+      <c r="J161" s="5" t="s">
+        <v>229</v>
+      </c>
       <c r="K161" s="5"/>
-      <c r="L161" s="7"/>
-      <c r="M161" s="7"/>
+      <c r="L161" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M161" s="7" t="s">
+        <v>230</v>
+      </c>
       <c r="N161" s="7"/>
       <c r="O161" s="2"/>
       <c r="P161" s="7"/>
@@ -9321,17 +9371,37 @@
     </row>
     <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18">
       <c r="A162" s="49"/>
-      <c r="B162" s="7"/>
-      <c r="C162" s="80"/>
-      <c r="D162" s="80"/>
-      <c r="E162" s="7"/>
-      <c r="F162" s="80"/>
-      <c r="G162" s="80"/>
-      <c r="H162" s="80"/>
-      <c r="I162" s="4"/>
-      <c r="J162" s="5"/>
+      <c r="B162" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C162" s="80" t="s">
+        <v>225</v>
+      </c>
+      <c r="D162" s="80" t="s">
+        <v>226</v>
+      </c>
+      <c r="E162" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="F162" s="80" t="s">
+        <v>228</v>
+      </c>
+      <c r="G162" s="80" t="s">
+        <v>29</v>
+      </c>
+      <c r="H162" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="I162" s="4">
+        <v>77</v>
+      </c>
+      <c r="J162" s="5" t="s">
+        <v>232</v>
+      </c>
       <c r="K162" s="5"/>
-      <c r="L162" s="7"/>
+      <c r="L162" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="M162" s="7"/>
       <c r="N162" s="7"/>
       <c r="O162" s="2"/>
@@ -9343,17 +9413,37 @@
     </row>
     <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18">
       <c r="A163" s="49"/>
-      <c r="B163" s="7"/>
-      <c r="C163" s="80"/>
-      <c r="D163" s="80"/>
-      <c r="E163" s="7"/>
-      <c r="F163" s="80"/>
-      <c r="G163" s="80"/>
-      <c r="H163" s="80"/>
-      <c r="I163" s="4"/>
-      <c r="J163" s="5"/>
+      <c r="B163" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C163" s="80" t="s">
+        <v>225</v>
+      </c>
+      <c r="D163" s="80" t="s">
+        <v>226</v>
+      </c>
+      <c r="E163" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="F163" s="80" t="s">
+        <v>228</v>
+      </c>
+      <c r="G163" s="80" t="s">
+        <v>29</v>
+      </c>
+      <c r="H163" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="I163" s="4">
+        <v>4</v>
+      </c>
+      <c r="J163" s="5" t="s">
+        <v>234</v>
+      </c>
       <c r="K163" s="5"/>
-      <c r="L163" s="7"/>
+      <c r="L163" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="M163" s="7"/>
       <c r="N163" s="7"/>
       <c r="O163" s="2"/>
@@ -9365,17 +9455,37 @@
     </row>
     <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18">
       <c r="A164" s="49"/>
-      <c r="B164" s="7"/>
-      <c r="C164" s="80"/>
-      <c r="D164" s="80"/>
-      <c r="E164" s="7"/>
-      <c r="F164" s="80"/>
-      <c r="G164" s="80"/>
-      <c r="H164" s="80"/>
-      <c r="I164" s="4"/>
-      <c r="J164" s="5"/>
+      <c r="B164" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C164" s="80" t="s">
+        <v>225</v>
+      </c>
+      <c r="D164" s="80" t="s">
+        <v>226</v>
+      </c>
+      <c r="E164" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="F164" s="80" t="s">
+        <v>235</v>
+      </c>
+      <c r="G164" s="80" t="s">
+        <v>29</v>
+      </c>
+      <c r="H164" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="I164" s="4">
+        <v>298</v>
+      </c>
+      <c r="J164" s="5" t="s">
+        <v>236</v>
+      </c>
       <c r="K164" s="5"/>
-      <c r="L164" s="7"/>
+      <c r="L164" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="M164" s="7"/>
       <c r="N164" s="7"/>
       <c r="O164" s="2"/>
@@ -9387,17 +9497,37 @@
     </row>
     <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="18">
       <c r="A165" s="49"/>
-      <c r="B165" s="7"/>
-      <c r="C165" s="80"/>
-      <c r="D165" s="80"/>
-      <c r="E165" s="7"/>
-      <c r="F165" s="80"/>
-      <c r="G165" s="80"/>
-      <c r="H165" s="80"/>
-      <c r="I165" s="4"/>
-      <c r="J165" s="5"/>
+      <c r="B165" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C165" s="80" t="s">
+        <v>225</v>
+      </c>
+      <c r="D165" s="80" t="s">
+        <v>226</v>
+      </c>
+      <c r="E165" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="F165" s="80" t="s">
+        <v>235</v>
+      </c>
+      <c r="G165" s="80" t="s">
+        <v>29</v>
+      </c>
+      <c r="H165" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="I165" s="4">
+        <v>77</v>
+      </c>
+      <c r="J165" s="5" t="s">
+        <v>232</v>
+      </c>
       <c r="K165" s="5"/>
-      <c r="L165" s="7"/>
+      <c r="L165" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="M165" s="7"/>
       <c r="N165" s="7"/>
       <c r="O165" s="2"/>
@@ -9409,17 +9539,37 @@
     </row>
     <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18">
       <c r="A166" s="49"/>
-      <c r="B166" s="7"/>
-      <c r="C166" s="80"/>
-      <c r="D166" s="80"/>
-      <c r="E166" s="7"/>
-      <c r="F166" s="80"/>
-      <c r="G166" s="80"/>
-      <c r="H166" s="80"/>
-      <c r="I166" s="4"/>
-      <c r="J166" s="5"/>
+      <c r="B166" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C166" s="80" t="s">
+        <v>225</v>
+      </c>
+      <c r="D166" s="80" t="s">
+        <v>226</v>
+      </c>
+      <c r="E166" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="F166" s="80" t="s">
+        <v>235</v>
+      </c>
+      <c r="G166" s="80" t="s">
+        <v>29</v>
+      </c>
+      <c r="H166" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="I166" s="4">
+        <v>4</v>
+      </c>
+      <c r="J166" s="5" t="s">
+        <v>237</v>
+      </c>
       <c r="K166" s="5"/>
-      <c r="L166" s="7"/>
+      <c r="L166" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="M166" s="7"/>
       <c r="N166" s="7"/>
       <c r="O166" s="2"/>
@@ -9431,17 +9581,37 @@
     </row>
     <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18">
       <c r="A167" s="49"/>
-      <c r="B167" s="7"/>
-      <c r="C167" s="80"/>
-      <c r="D167" s="80"/>
-      <c r="E167" s="7"/>
-      <c r="F167" s="80"/>
-      <c r="G167" s="80"/>
-      <c r="H167" s="80"/>
-      <c r="I167" s="4"/>
-      <c r="J167" s="5"/>
+      <c r="B167" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C167" s="80" t="s">
+        <v>225</v>
+      </c>
+      <c r="D167" s="80" t="s">
+        <v>226</v>
+      </c>
+      <c r="E167" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="F167" s="80" t="s">
+        <v>79</v>
+      </c>
+      <c r="G167" s="80" t="s">
+        <v>29</v>
+      </c>
+      <c r="H167" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="I167" s="4">
+        <v>298</v>
+      </c>
+      <c r="J167" s="5">
+        <v>16</v>
+      </c>
       <c r="K167" s="5"/>
-      <c r="L167" s="7"/>
+      <c r="L167" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="M167" s="7"/>
       <c r="N167" s="7"/>
       <c r="O167" s="2"/>
@@ -9453,17 +9623,37 @@
     </row>
     <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18">
       <c r="A168" s="49"/>
-      <c r="B168" s="7"/>
-      <c r="C168" s="80"/>
-      <c r="D168" s="80"/>
-      <c r="E168" s="7"/>
-      <c r="F168" s="80"/>
-      <c r="G168" s="80"/>
-      <c r="H168" s="80"/>
-      <c r="I168" s="4"/>
-      <c r="J168" s="5"/>
+      <c r="B168" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C168" s="80" t="s">
+        <v>225</v>
+      </c>
+      <c r="D168" s="80" t="s">
+        <v>226</v>
+      </c>
+      <c r="E168" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="F168" s="80" t="s">
+        <v>79</v>
+      </c>
+      <c r="G168" s="80" t="s">
+        <v>29</v>
+      </c>
+      <c r="H168" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="I168" s="4">
+        <v>77</v>
+      </c>
+      <c r="J168" s="5">
+        <v>18</v>
+      </c>
       <c r="K168" s="5"/>
-      <c r="L168" s="7"/>
+      <c r="L168" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="M168" s="7"/>
       <c r="N168" s="7"/>
       <c r="O168" s="2"/>
@@ -9475,17 +9665,37 @@
     </row>
     <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="18">
       <c r="A169" s="49"/>
-      <c r="B169" s="7"/>
-      <c r="C169" s="80"/>
-      <c r="D169" s="80"/>
-      <c r="E169" s="7"/>
-      <c r="F169" s="80"/>
-      <c r="G169" s="80"/>
-      <c r="H169" s="80"/>
-      <c r="I169" s="4"/>
-      <c r="J169" s="5"/>
+      <c r="B169" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C169" s="80" t="s">
+        <v>225</v>
+      </c>
+      <c r="D169" s="80" t="s">
+        <v>226</v>
+      </c>
+      <c r="E169" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="F169" s="80" t="s">
+        <v>79</v>
+      </c>
+      <c r="G169" s="80" t="s">
+        <v>29</v>
+      </c>
+      <c r="H169" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="I169" s="4">
+        <v>4</v>
+      </c>
+      <c r="J169" s="5">
+        <v>19.5</v>
+      </c>
       <c r="K169" s="5"/>
-      <c r="L169" s="7"/>
+      <c r="L169" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="M169" s="7"/>
       <c r="N169" s="7"/>
       <c r="O169" s="2"/>

</xml_diff>

<commit_message>
- fix missing reference data for `10.1038/s41563-024-01871-7`
</commit_message>
<xml_diff>
--- a/DuctilitySearch_Feb24.xlsx
+++ b/DuctilitySearch_Feb24.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1583" uniqueCount="239">
   <si>
     <t>Metadata</t>
   </si>
@@ -798,6 +798,9 @@
   </si>
   <si>
     <t>F2</t>
+  </si>
+  <si>
+    <t>10.1038/s41563-024-01871-7</t>
   </si>
   <si>
     <t>strain rate 0.5e-3; liquid nitrogen</t>
@@ -8933,7 +8936,7 @@
       <c r="S152" s="2"/>
       <c r="T152" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
       <c r="A153" s="49">
         <v>8</v>
       </c>
@@ -8983,7 +8986,7 @@
       <c r="S153" s="2"/>
       <c r="T153" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
       <c r="A154" s="49">
         <v>8</v>
       </c>
@@ -9033,7 +9036,7 @@
       <c r="S154" s="2"/>
       <c r="T154" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
       <c r="A155" s="49">
         <v>8</v>
       </c>
@@ -9083,7 +9086,7 @@
       <c r="S155" s="2"/>
       <c r="T155" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75">
       <c r="A156" s="49">
         <v>8</v>
       </c>
@@ -9131,7 +9134,7 @@
       <c r="S156" s="2"/>
       <c r="T156" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75">
       <c r="A157" s="49">
         <v>8</v>
       </c>
@@ -9179,7 +9182,7 @@
       <c r="S157" s="2"/>
       <c r="T157" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
       <c r="A158" s="49">
         <v>8</v>
       </c>
@@ -9227,7 +9230,7 @@
       <c r="S158" s="2"/>
       <c r="T158" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75">
       <c r="A159" s="49">
         <v>8</v>
       </c>
@@ -9275,7 +9278,7 @@
       <c r="S159" s="2"/>
       <c r="T159" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75">
       <c r="A160" s="49">
         <v>8</v>
       </c>
@@ -9323,26 +9326,26 @@
       <c r="S160" s="2"/>
       <c r="T160" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="20.25">
       <c r="A161" s="49">
         <v>9</v>
       </c>
-      <c r="B161" s="7" t="s">
+      <c r="B161" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="C161" s="80" t="s">
+      <c r="C161" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D161" s="80" t="s">
+      <c r="D161" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="E161" s="7" t="s">
+      <c r="E161" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="F161" s="80" t="s">
+      <c r="F161" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="G161" s="80" t="s">
+      <c r="G161" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H161" s="3" t="s">
@@ -9355,13 +9358,15 @@
         <v>229</v>
       </c>
       <c r="K161" s="5"/>
-      <c r="L161" s="7" t="s">
+      <c r="L161" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M161" s="7" t="s">
+      <c r="M161" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="N161" s="7"/>
+      <c r="N161" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="O161" s="2"/>
       <c r="P161" s="7"/>
       <c r="Q161" s="2"/>
@@ -9369,41 +9374,47 @@
       <c r="S161" s="2"/>
       <c r="T161" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18">
-      <c r="A162" s="49"/>
-      <c r="B162" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="20.25">
+      <c r="A162" s="49">
+        <v>9</v>
+      </c>
+      <c r="B162" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="C162" s="80" t="s">
+      <c r="C162" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D162" s="80" t="s">
+      <c r="D162" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="E162" s="7" t="s">
+      <c r="E162" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="F162" s="80" t="s">
+      <c r="F162" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="G162" s="80" t="s">
+      <c r="G162" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H162" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I162" s="4">
         <v>77</v>
       </c>
       <c r="J162" s="5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="K162" s="5"/>
-      <c r="L162" s="7" t="s">
+      <c r="L162" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M162" s="7"/>
-      <c r="N162" s="7"/>
+      <c r="M162" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="N162" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="O162" s="2"/>
       <c r="P162" s="7"/>
       <c r="Q162" s="2"/>
@@ -9411,41 +9422,47 @@
       <c r="S162" s="2"/>
       <c r="T162" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18">
-      <c r="A163" s="49"/>
-      <c r="B163" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="20.25">
+      <c r="A163" s="49">
+        <v>9</v>
+      </c>
+      <c r="B163" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="C163" s="80" t="s">
+      <c r="C163" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D163" s="80" t="s">
+      <c r="D163" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="E163" s="7" t="s">
+      <c r="E163" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="F163" s="80" t="s">
+      <c r="F163" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="G163" s="80" t="s">
+      <c r="G163" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H163" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="I163" s="4">
         <v>4</v>
       </c>
       <c r="J163" s="5" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="K163" s="5"/>
-      <c r="L163" s="7" t="s">
+      <c r="L163" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M163" s="7"/>
-      <c r="N163" s="7"/>
+      <c r="M163" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="N163" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="O163" s="2"/>
       <c r="P163" s="7"/>
       <c r="Q163" s="2"/>
@@ -9453,24 +9470,26 @@
       <c r="S163" s="2"/>
       <c r="T163" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18">
-      <c r="A164" s="49"/>
-      <c r="B164" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="20.25">
+      <c r="A164" s="49">
+        <v>9</v>
+      </c>
+      <c r="B164" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="C164" s="80" t="s">
+      <c r="C164" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D164" s="80" t="s">
+      <c r="D164" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="E164" s="7" t="s">
+      <c r="E164" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="F164" s="80" t="s">
-        <v>235</v>
-      </c>
-      <c r="G164" s="80" t="s">
+      <c r="F164" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="G164" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H164" s="3" t="s">
@@ -9480,14 +9499,18 @@
         <v>298</v>
       </c>
       <c r="J164" s="5" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="K164" s="5"/>
-      <c r="L164" s="7" t="s">
+      <c r="L164" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M164" s="7"/>
-      <c r="N164" s="7"/>
+      <c r="M164" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="N164" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="O164" s="2"/>
       <c r="P164" s="7"/>
       <c r="Q164" s="2"/>
@@ -9495,41 +9518,47 @@
       <c r="S164" s="2"/>
       <c r="T164" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="18">
-      <c r="A165" s="49"/>
-      <c r="B165" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="20.25">
+      <c r="A165" s="49">
+        <v>9</v>
+      </c>
+      <c r="B165" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="C165" s="80" t="s">
+      <c r="C165" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D165" s="80" t="s">
+      <c r="D165" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="E165" s="7" t="s">
+      <c r="E165" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="F165" s="80" t="s">
-        <v>235</v>
-      </c>
-      <c r="G165" s="80" t="s">
+      <c r="F165" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="G165" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H165" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I165" s="4">
         <v>77</v>
       </c>
       <c r="J165" s="5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="K165" s="5"/>
-      <c r="L165" s="7" t="s">
+      <c r="L165" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M165" s="7"/>
-      <c r="N165" s="7"/>
+      <c r="M165" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="N165" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="O165" s="2"/>
       <c r="P165" s="7"/>
       <c r="Q165" s="2"/>
@@ -9537,41 +9566,47 @@
       <c r="S165" s="2"/>
       <c r="T165" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18">
-      <c r="A166" s="49"/>
-      <c r="B166" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="20.25">
+      <c r="A166" s="49">
+        <v>9</v>
+      </c>
+      <c r="B166" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="C166" s="80" t="s">
+      <c r="C166" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D166" s="80" t="s">
+      <c r="D166" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="E166" s="7" t="s">
+      <c r="E166" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="F166" s="80" t="s">
-        <v>235</v>
-      </c>
-      <c r="G166" s="80" t="s">
+      <c r="F166" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="G166" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H166" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="I166" s="4">
         <v>4</v>
       </c>
       <c r="J166" s="5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="K166" s="5"/>
-      <c r="L166" s="7" t="s">
+      <c r="L166" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M166" s="7"/>
-      <c r="N166" s="7"/>
+      <c r="M166" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="N166" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="O166" s="2"/>
       <c r="P166" s="7"/>
       <c r="Q166" s="2"/>
@@ -9579,24 +9614,26 @@
       <c r="S166" s="2"/>
       <c r="T166" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18">
-      <c r="A167" s="49"/>
-      <c r="B167" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="20.25">
+      <c r="A167" s="49">
+        <v>9</v>
+      </c>
+      <c r="B167" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="C167" s="80" t="s">
+      <c r="C167" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D167" s="80" t="s">
+      <c r="D167" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="E167" s="7" t="s">
+      <c r="E167" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="F167" s="80" t="s">
+      <c r="F167" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G167" s="80" t="s">
+      <c r="G167" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H167" s="3" t="s">
@@ -9609,11 +9646,15 @@
         <v>16</v>
       </c>
       <c r="K167" s="5"/>
-      <c r="L167" s="7" t="s">
+      <c r="L167" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M167" s="7"/>
-      <c r="N167" s="7"/>
+      <c r="M167" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="N167" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="O167" s="2"/>
       <c r="P167" s="7"/>
       <c r="Q167" s="2"/>
@@ -9621,28 +9662,30 @@
       <c r="S167" s="2"/>
       <c r="T167" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18">
-      <c r="A168" s="49"/>
-      <c r="B168" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="20.25">
+      <c r="A168" s="49">
+        <v>9</v>
+      </c>
+      <c r="B168" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="C168" s="80" t="s">
+      <c r="C168" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D168" s="80" t="s">
+      <c r="D168" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="E168" s="7" t="s">
+      <c r="E168" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="F168" s="80" t="s">
+      <c r="F168" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G168" s="80" t="s">
+      <c r="G168" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H168" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I168" s="4">
         <v>77</v>
@@ -9651,11 +9694,15 @@
         <v>18</v>
       </c>
       <c r="K168" s="5"/>
-      <c r="L168" s="7" t="s">
+      <c r="L168" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M168" s="7"/>
-      <c r="N168" s="7"/>
+      <c r="M168" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="N168" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="O168" s="2"/>
       <c r="P168" s="7"/>
       <c r="Q168" s="2"/>
@@ -9663,28 +9710,30 @@
       <c r="S168" s="2"/>
       <c r="T168" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="18">
-      <c r="A169" s="49"/>
-      <c r="B169" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="20.25">
+      <c r="A169" s="49">
+        <v>9</v>
+      </c>
+      <c r="B169" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="C169" s="80" t="s">
+      <c r="C169" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D169" s="80" t="s">
+      <c r="D169" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="E169" s="7" t="s">
+      <c r="E169" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="F169" s="80" t="s">
+      <c r="F169" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G169" s="80" t="s">
+      <c r="G169" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H169" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="I169" s="4">
         <v>4</v>
@@ -9693,11 +9742,15 @@
         <v>19.5</v>
       </c>
       <c r="K169" s="5"/>
-      <c r="L169" s="7" t="s">
+      <c r="L169" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M169" s="7"/>
-      <c r="N169" s="7"/>
+      <c r="M169" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="N169" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="O169" s="2"/>
       <c r="P169" s="7"/>
       <c r="Q169" s="2"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.ijrmhm.2020.105405`
</commit_message>
<xml_diff>
--- a/DuctilitySearch_Feb24.xlsx
+++ b/DuctilitySearch_Feb24.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1583" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1742" uniqueCount="261">
   <si>
     <t>Metadata</t>
   </si>
@@ -823,6 +823,73 @@
   <si>
     <t>2.35e9</t>
   </si>
+  <si>
+    <t>Hf0.5 Mo0.5 Nb Ti Zr Cr0.1</t>
+  </si>
+  <si>
+    <t>mid-button cut</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>10.1016/j.ijrmhm.2020.105405</t>
+  </si>
+  <si>
+    <t>Hf0.5 Mo0.5 Nb Ti Zr Cr0.2</t>
+  </si>
+  <si>
+    <t>Hf0.5 Mo0.5 Nb Ti Zr Cr0.3</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>Hf0.5 Mo0.5 Nb Ti Zr Cr0.4</t>
+  </si>
+  <si>
+    <t>BCC+laves</t>
+  </si>
+  <si>
+    <t>CrMoZr phase Fd-3m Cu2Mg-typed Laves phase; mid-button cut</t>
+  </si>
+  <si>
+    <t>Hf0.5 Mo0.5 Nb Ti Zr Cr0.5</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>homogenized at 1100C for 10h; homogenization stabilizes the CrMoZr phase Fd-3m Cu2Mg-typed Laves phase
+; mid-button cut</t>
+  </si>
+  <si>
+    <t>1275e6</t>
+  </si>
+  <si>
+    <t>75e6</t>
+  </si>
+  <si>
+    <t>1350e6</t>
+  </si>
+  <si>
+    <t>1300e6</t>
+  </si>
+  <si>
+    <t>1475e6</t>
+  </si>
+  <si>
+    <t>1875e6</t>
+  </si>
+  <si>
+    <t>1675e6</t>
+  </si>
+  <si>
+    <t>1600e6</t>
+  </si>
 </sst>
 </file>
 
@@ -832,7 +899,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.000000"/>
     <numFmt numFmtId="165" formatCode="#,##0.00000000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -895,6 +962,12 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1408,7 +1481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="94">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1661,6 +1734,15 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1982,32 +2064,32 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T425"/>
+  <dimension ref="A1:T424"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="85" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="86" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="87" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="87" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="86" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="87" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="87" width="19.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="87" width="21.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="88" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="89" width="25.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="89" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="90" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="90" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="90" width="34.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="86" width="39.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="85" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="86" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="86" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="86" width="17.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="86" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="88" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="89" width="31.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="90" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="90" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="89" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="90" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="90" width="19.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="90" width="21.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="91" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="92" width="25.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="92" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="93" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="93" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="93" width="34.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="89" width="39.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="88" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="89" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="89" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="89" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="89" width="17.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
@@ -9759,20 +9841,46 @@
       <c r="T169" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="18">
-      <c r="A170" s="49"/>
-      <c r="B170" s="7"/>
-      <c r="C170" s="80"/>
-      <c r="D170" s="80"/>
-      <c r="E170" s="7"/>
-      <c r="F170" s="80"/>
-      <c r="G170" s="80"/>
+      <c r="A170" s="49">
+        <v>10</v>
+      </c>
+      <c r="B170" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="C170" s="80" t="s">
+        <v>65</v>
+      </c>
+      <c r="D170" s="80" t="s">
+        <v>66</v>
+      </c>
+      <c r="E170" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="F170" s="80" t="s">
+        <v>107</v>
+      </c>
+      <c r="G170" s="80" t="s">
+        <v>29</v>
+      </c>
       <c r="H170" s="80"/>
-      <c r="I170" s="4"/>
-      <c r="J170" s="5"/>
-      <c r="K170" s="5"/>
-      <c r="L170" s="7"/>
-      <c r="M170" s="7"/>
-      <c r="N170" s="7"/>
+      <c r="I170" s="4">
+        <v>298</v>
+      </c>
+      <c r="J170" s="5">
+        <v>37.5</v>
+      </c>
+      <c r="K170" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="L170" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="M170" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="N170" s="7" t="s">
+        <v>242</v>
+      </c>
       <c r="O170" s="2"/>
       <c r="P170" s="7"/>
       <c r="Q170" s="2"/>
@@ -9781,20 +9889,46 @@
       <c r="T170" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="18">
-      <c r="A171" s="49"/>
-      <c r="B171" s="7"/>
-      <c r="C171" s="80"/>
-      <c r="D171" s="80"/>
-      <c r="E171" s="7"/>
-      <c r="F171" s="80"/>
-      <c r="G171" s="80"/>
+      <c r="A171" s="49">
+        <v>10</v>
+      </c>
+      <c r="B171" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C171" s="80" t="s">
+        <v>65</v>
+      </c>
+      <c r="D171" s="80" t="s">
+        <v>66</v>
+      </c>
+      <c r="E171" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="F171" s="80" t="s">
+        <v>107</v>
+      </c>
+      <c r="G171" s="80" t="s">
+        <v>29</v>
+      </c>
       <c r="H171" s="80"/>
-      <c r="I171" s="4"/>
-      <c r="J171" s="5"/>
-      <c r="K171" s="5"/>
-      <c r="L171" s="7"/>
-      <c r="M171" s="7"/>
-      <c r="N171" s="7"/>
+      <c r="I171" s="4">
+        <v>298</v>
+      </c>
+      <c r="J171" s="5">
+        <v>22</v>
+      </c>
+      <c r="K171" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="L171" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="M171" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="N171" s="7" t="s">
+        <v>242</v>
+      </c>
       <c r="O171" s="2"/>
       <c r="P171" s="7"/>
       <c r="Q171" s="2"/>
@@ -9803,20 +9937,38 @@
       <c r="T171" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="18">
-      <c r="A172" s="49"/>
-      <c r="B172" s="7"/>
-      <c r="C172" s="80"/>
-      <c r="D172" s="80"/>
-      <c r="E172" s="7"/>
-      <c r="F172" s="80"/>
-      <c r="G172" s="80"/>
+      <c r="A172" s="49">
+        <v>10</v>
+      </c>
+      <c r="B172" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C172" s="80" t="s">
+        <v>65</v>
+      </c>
+      <c r="D172" s="80" t="s">
+        <v>66</v>
+      </c>
+      <c r="E172" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="F172" s="85" t="s">
+        <v>245</v>
+      </c>
+      <c r="G172" s="85" t="s">
+        <v>245</v>
+      </c>
       <c r="H172" s="80"/>
       <c r="I172" s="4"/>
       <c r="J172" s="5"/>
       <c r="K172" s="5"/>
       <c r="L172" s="7"/>
-      <c r="M172" s="7"/>
-      <c r="N172" s="7"/>
+      <c r="M172" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="N172" s="7" t="s">
+        <v>242</v>
+      </c>
       <c r="O172" s="2"/>
       <c r="P172" s="7"/>
       <c r="Q172" s="2"/>
@@ -9825,20 +9977,46 @@
       <c r="T172" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18">
-      <c r="A173" s="49"/>
-      <c r="B173" s="7"/>
-      <c r="C173" s="80"/>
-      <c r="D173" s="80"/>
-      <c r="E173" s="7"/>
-      <c r="F173" s="80"/>
-      <c r="G173" s="80"/>
+      <c r="A173" s="49">
+        <v>10</v>
+      </c>
+      <c r="B173" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="C173" s="80" t="s">
+        <v>248</v>
+      </c>
+      <c r="D173" s="80" t="s">
+        <v>66</v>
+      </c>
+      <c r="E173" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F173" s="80" t="s">
+        <v>107</v>
+      </c>
+      <c r="G173" s="80" t="s">
+        <v>29</v>
+      </c>
       <c r="H173" s="80"/>
-      <c r="I173" s="4"/>
-      <c r="J173" s="5"/>
-      <c r="K173" s="5"/>
-      <c r="L173" s="7"/>
-      <c r="M173" s="7"/>
-      <c r="N173" s="7"/>
+      <c r="I173" s="4">
+        <v>298</v>
+      </c>
+      <c r="J173" s="5">
+        <v>17.5</v>
+      </c>
+      <c r="K173" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="L173" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="M173" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="N173" s="7" t="s">
+        <v>242</v>
+      </c>
       <c r="O173" s="2"/>
       <c r="P173" s="7"/>
       <c r="Q173" s="2"/>
@@ -9847,20 +10025,46 @@
       <c r="T173" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18">
-      <c r="A174" s="49"/>
-      <c r="B174" s="7"/>
-      <c r="C174" s="80"/>
-      <c r="D174" s="80"/>
-      <c r="E174" s="7"/>
-      <c r="F174" s="80"/>
-      <c r="G174" s="80"/>
+      <c r="A174" s="49">
+        <v>10</v>
+      </c>
+      <c r="B174" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="C174" s="80" t="s">
+        <v>248</v>
+      </c>
+      <c r="D174" s="80" t="s">
+        <v>66</v>
+      </c>
+      <c r="E174" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F174" s="80" t="s">
+        <v>107</v>
+      </c>
+      <c r="G174" s="80" t="s">
+        <v>29</v>
+      </c>
       <c r="H174" s="80"/>
-      <c r="I174" s="4"/>
-      <c r="J174" s="5"/>
-      <c r="K174" s="5"/>
-      <c r="L174" s="7"/>
-      <c r="M174" s="7"/>
-      <c r="N174" s="7"/>
+      <c r="I174" s="4">
+        <v>298</v>
+      </c>
+      <c r="J174" s="5">
+        <v>11</v>
+      </c>
+      <c r="K174" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="L174" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="M174" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="N174" s="7" t="s">
+        <v>242</v>
+      </c>
       <c r="O174" s="2"/>
       <c r="P174" s="7"/>
       <c r="Q174" s="2"/>
@@ -9869,20 +10073,46 @@
       <c r="T174" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18">
-      <c r="A175" s="49"/>
-      <c r="B175" s="7"/>
-      <c r="C175" s="80"/>
-      <c r="D175" s="80"/>
-      <c r="E175" s="7"/>
-      <c r="F175" s="80"/>
-      <c r="G175" s="80"/>
+      <c r="A175" s="49">
+        <v>10</v>
+      </c>
+      <c r="B175" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C175" s="80" t="s">
+        <v>248</v>
+      </c>
+      <c r="D175" s="80" t="s">
+        <v>251</v>
+      </c>
+      <c r="E175" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="F175" s="80" t="s">
+        <v>107</v>
+      </c>
+      <c r="G175" s="80" t="s">
+        <v>29</v>
+      </c>
       <c r="H175" s="80"/>
-      <c r="I175" s="4"/>
-      <c r="J175" s="5"/>
-      <c r="K175" s="5"/>
-      <c r="L175" s="7"/>
-      <c r="M175" s="7"/>
-      <c r="N175" s="7"/>
+      <c r="I175" s="4">
+        <v>298</v>
+      </c>
+      <c r="J175" s="5">
+        <v>19</v>
+      </c>
+      <c r="K175" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="L175" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="M175" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="N175" s="7" t="s">
+        <v>242</v>
+      </c>
       <c r="O175" s="2"/>
       <c r="P175" s="7"/>
       <c r="Q175" s="2"/>
@@ -9891,20 +10121,46 @@
       <c r="T175" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18">
-      <c r="A176" s="49"/>
-      <c r="B176" s="7"/>
-      <c r="C176" s="80"/>
-      <c r="D176" s="80"/>
-      <c r="E176" s="7"/>
-      <c r="F176" s="80"/>
-      <c r="G176" s="80"/>
+      <c r="A176" s="49">
+        <v>10</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C176" s="86" t="s">
+        <v>65</v>
+      </c>
+      <c r="D176" s="86" t="s">
+        <v>66</v>
+      </c>
+      <c r="E176" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F176" s="86" t="s">
+        <v>88</v>
+      </c>
+      <c r="G176" s="80" t="s">
+        <v>29</v>
+      </c>
       <c r="H176" s="80"/>
-      <c r="I176" s="4"/>
-      <c r="J176" s="5"/>
-      <c r="K176" s="5"/>
-      <c r="L176" s="7"/>
-      <c r="M176" s="7"/>
-      <c r="N176" s="7"/>
+      <c r="I176" s="4">
+        <v>298</v>
+      </c>
+      <c r="J176" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="K176" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="L176" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M176" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="N176" s="7" t="s">
+        <v>242</v>
+      </c>
       <c r="O176" s="2"/>
       <c r="P176" s="7"/>
       <c r="Q176" s="2"/>
@@ -9913,20 +10169,46 @@
       <c r="T176" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18">
-      <c r="A177" s="49"/>
-      <c r="B177" s="7"/>
-      <c r="C177" s="80"/>
-      <c r="D177" s="80"/>
-      <c r="E177" s="7"/>
-      <c r="F177" s="80"/>
-      <c r="G177" s="80"/>
+      <c r="A177" s="49">
+        <v>10</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C177" s="86" t="s">
+        <v>65</v>
+      </c>
+      <c r="D177" s="86" t="s">
+        <v>66</v>
+      </c>
+      <c r="E177" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F177" s="86" t="s">
+        <v>88</v>
+      </c>
+      <c r="G177" s="80" t="s">
+        <v>29</v>
+      </c>
       <c r="H177" s="80"/>
-      <c r="I177" s="4"/>
-      <c r="J177" s="5"/>
-      <c r="K177" s="5"/>
-      <c r="L177" s="7"/>
-      <c r="M177" s="7"/>
-      <c r="N177" s="7"/>
+      <c r="I177" s="4">
+        <v>298</v>
+      </c>
+      <c r="J177" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="K177" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="L177" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M177" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="N177" s="7" t="s">
+        <v>242</v>
+      </c>
       <c r="O177" s="2"/>
       <c r="P177" s="7"/>
       <c r="Q177" s="2"/>
@@ -9935,20 +10217,46 @@
       <c r="T177" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18">
-      <c r="A178" s="49"/>
-      <c r="B178" s="7"/>
-      <c r="C178" s="80"/>
-      <c r="D178" s="80"/>
-      <c r="E178" s="7"/>
-      <c r="F178" s="80"/>
-      <c r="G178" s="80"/>
+      <c r="A178" s="49">
+        <v>10</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C178" s="86" t="s">
+        <v>248</v>
+      </c>
+      <c r="D178" s="86" t="s">
+        <v>66</v>
+      </c>
+      <c r="E178" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F178" s="86" t="s">
+        <v>88</v>
+      </c>
+      <c r="G178" s="80" t="s">
+        <v>29</v>
+      </c>
       <c r="H178" s="80"/>
-      <c r="I178" s="4"/>
-      <c r="J178" s="5"/>
-      <c r="K178" s="5"/>
-      <c r="L178" s="7"/>
-      <c r="M178" s="7"/>
-      <c r="N178" s="7"/>
+      <c r="I178" s="4">
+        <v>298</v>
+      </c>
+      <c r="J178" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="K178" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="L178" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M178" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="N178" s="7" t="s">
+        <v>242</v>
+      </c>
       <c r="O178" s="2"/>
       <c r="P178" s="7"/>
       <c r="Q178" s="2"/>
@@ -9957,20 +10265,46 @@
       <c r="T178" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18">
-      <c r="A179" s="49"/>
-      <c r="B179" s="7"/>
-      <c r="C179" s="80"/>
-      <c r="D179" s="80"/>
-      <c r="E179" s="7"/>
-      <c r="F179" s="80"/>
-      <c r="G179" s="80"/>
+      <c r="A179" s="49">
+        <v>10</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C179" s="86" t="s">
+        <v>248</v>
+      </c>
+      <c r="D179" s="86" t="s">
+        <v>66</v>
+      </c>
+      <c r="E179" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F179" s="86" t="s">
+        <v>88</v>
+      </c>
+      <c r="G179" s="80" t="s">
+        <v>29</v>
+      </c>
       <c r="H179" s="80"/>
-      <c r="I179" s="4"/>
-      <c r="J179" s="5"/>
-      <c r="K179" s="5"/>
-      <c r="L179" s="7"/>
-      <c r="M179" s="7"/>
-      <c r="N179" s="7"/>
+      <c r="I179" s="4">
+        <v>298</v>
+      </c>
+      <c r="J179" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="K179" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="L179" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M179" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="N179" s="7" t="s">
+        <v>242</v>
+      </c>
       <c r="O179" s="2"/>
       <c r="P179" s="7"/>
       <c r="Q179" s="2"/>
@@ -9978,21 +10312,47 @@
       <c r="S179" s="2"/>
       <c r="T179" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18">
-      <c r="A180" s="49"/>
-      <c r="B180" s="7"/>
-      <c r="C180" s="80"/>
-      <c r="D180" s="80"/>
-      <c r="E180" s="7"/>
-      <c r="F180" s="80"/>
-      <c r="G180" s="80"/>
+    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="17.25">
+      <c r="A180" s="49">
+        <v>10</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C180" s="86" t="s">
+        <v>248</v>
+      </c>
+      <c r="D180" s="86" t="s">
+        <v>251</v>
+      </c>
+      <c r="E180" s="87" t="s">
+        <v>252</v>
+      </c>
+      <c r="F180" s="86" t="s">
+        <v>88</v>
+      </c>
+      <c r="G180" s="80" t="s">
+        <v>29</v>
+      </c>
       <c r="H180" s="80"/>
-      <c r="I180" s="4"/>
-      <c r="J180" s="5"/>
-      <c r="K180" s="5"/>
-      <c r="L180" s="7"/>
-      <c r="M180" s="7"/>
-      <c r="N180" s="7"/>
+      <c r="I180" s="4">
+        <v>298</v>
+      </c>
+      <c r="J180" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="K180" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="L180" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M180" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="N180" s="7" t="s">
+        <v>242</v>
+      </c>
       <c r="O180" s="2"/>
       <c r="P180" s="7"/>
       <c r="Q180" s="2"/>
@@ -10001,20 +10361,46 @@
       <c r="T180" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="18">
-      <c r="A181" s="49"/>
-      <c r="B181" s="7"/>
-      <c r="C181" s="80"/>
-      <c r="D181" s="80"/>
-      <c r="E181" s="7"/>
-      <c r="F181" s="80"/>
-      <c r="G181" s="80"/>
+      <c r="A181" s="49">
+        <v>10</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C181" s="86" t="s">
+        <v>65</v>
+      </c>
+      <c r="D181" s="86" t="s">
+        <v>66</v>
+      </c>
+      <c r="E181" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F181" s="86" t="s">
+        <v>149</v>
+      </c>
+      <c r="G181" s="80" t="s">
+        <v>29</v>
+      </c>
       <c r="H181" s="80"/>
-      <c r="I181" s="4"/>
-      <c r="J181" s="5"/>
-      <c r="K181" s="5"/>
-      <c r="L181" s="7"/>
-      <c r="M181" s="7"/>
-      <c r="N181" s="7"/>
+      <c r="I181" s="4">
+        <v>298</v>
+      </c>
+      <c r="J181" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="K181" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L181" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M181" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="N181" s="7" t="s">
+        <v>242</v>
+      </c>
       <c r="O181" s="2"/>
       <c r="P181" s="7"/>
       <c r="Q181" s="2"/>
@@ -10023,20 +10409,44 @@
       <c r="T181" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="18">
-      <c r="A182" s="49"/>
-      <c r="B182" s="7"/>
-      <c r="C182" s="80"/>
-      <c r="D182" s="80"/>
-      <c r="E182" s="7"/>
-      <c r="F182" s="80"/>
-      <c r="G182" s="80"/>
+      <c r="A182" s="49">
+        <v>10</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C182" s="86" t="s">
+        <v>65</v>
+      </c>
+      <c r="D182" s="86" t="s">
+        <v>66</v>
+      </c>
+      <c r="E182" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F182" s="86" t="s">
+        <v>149</v>
+      </c>
+      <c r="G182" s="80" t="s">
+        <v>29</v>
+      </c>
       <c r="H182" s="80"/>
-      <c r="I182" s="4"/>
-      <c r="J182" s="5"/>
+      <c r="I182" s="4">
+        <v>298</v>
+      </c>
+      <c r="J182" s="5" t="s">
+        <v>180</v>
+      </c>
       <c r="K182" s="5"/>
-      <c r="L182" s="7"/>
-      <c r="M182" s="7"/>
-      <c r="N182" s="7"/>
+      <c r="L182" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M182" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="N182" s="7" t="s">
+        <v>242</v>
+      </c>
       <c r="O182" s="2"/>
       <c r="P182" s="7"/>
       <c r="Q182" s="2"/>
@@ -10045,20 +10455,44 @@
       <c r="T182" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="18">
-      <c r="A183" s="49"/>
-      <c r="B183" s="7"/>
-      <c r="C183" s="80"/>
-      <c r="D183" s="80"/>
-      <c r="E183" s="7"/>
-      <c r="F183" s="80"/>
-      <c r="G183" s="80"/>
+      <c r="A183" s="49">
+        <v>10</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C183" s="86" t="s">
+        <v>248</v>
+      </c>
+      <c r="D183" s="86" t="s">
+        <v>66</v>
+      </c>
+      <c r="E183" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F183" s="86" t="s">
+        <v>149</v>
+      </c>
+      <c r="G183" s="80" t="s">
+        <v>29</v>
+      </c>
       <c r="H183" s="80"/>
-      <c r="I183" s="4"/>
-      <c r="J183" s="5"/>
+      <c r="I183" s="4">
+        <v>298</v>
+      </c>
+      <c r="J183" s="5" t="s">
+        <v>259</v>
+      </c>
       <c r="K183" s="5"/>
-      <c r="L183" s="7"/>
-      <c r="M183" s="7"/>
-      <c r="N183" s="7"/>
+      <c r="L183" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M183" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="N183" s="7" t="s">
+        <v>242</v>
+      </c>
       <c r="O183" s="2"/>
       <c r="P183" s="7"/>
       <c r="Q183" s="2"/>
@@ -10067,20 +10501,44 @@
       <c r="T183" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="18">
-      <c r="A184" s="49"/>
-      <c r="B184" s="7"/>
-      <c r="C184" s="80"/>
-      <c r="D184" s="80"/>
-      <c r="E184" s="7"/>
-      <c r="F184" s="80"/>
-      <c r="G184" s="80"/>
+      <c r="A184" s="49">
+        <v>10</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C184" s="86" t="s">
+        <v>248</v>
+      </c>
+      <c r="D184" s="86" t="s">
+        <v>66</v>
+      </c>
+      <c r="E184" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F184" s="86" t="s">
+        <v>149</v>
+      </c>
+      <c r="G184" s="80" t="s">
+        <v>29</v>
+      </c>
       <c r="H184" s="80"/>
-      <c r="I184" s="4"/>
-      <c r="J184" s="5"/>
+      <c r="I184" s="4">
+        <v>298</v>
+      </c>
+      <c r="J184" s="5" t="s">
+        <v>180</v>
+      </c>
       <c r="K184" s="5"/>
-      <c r="L184" s="7"/>
-      <c r="M184" s="7"/>
-      <c r="N184" s="7"/>
+      <c r="L184" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M184" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="N184" s="7" t="s">
+        <v>242</v>
+      </c>
       <c r="O184" s="2"/>
       <c r="P184" s="7"/>
       <c r="Q184" s="2"/>
@@ -10088,21 +10546,45 @@
       <c r="S184" s="2"/>
       <c r="T184" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="18">
-      <c r="A185" s="49"/>
-      <c r="B185" s="7"/>
-      <c r="C185" s="80"/>
-      <c r="D185" s="80"/>
-      <c r="E185" s="7"/>
-      <c r="F185" s="80"/>
-      <c r="G185" s="80"/>
+    <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="20.25">
+      <c r="A185" s="49">
+        <v>10</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C185" s="86" t="s">
+        <v>248</v>
+      </c>
+      <c r="D185" s="86" t="s">
+        <v>251</v>
+      </c>
+      <c r="E185" s="87" t="s">
+        <v>252</v>
+      </c>
+      <c r="F185" s="86" t="s">
+        <v>149</v>
+      </c>
+      <c r="G185" s="80" t="s">
+        <v>29</v>
+      </c>
       <c r="H185" s="80"/>
-      <c r="I185" s="4"/>
-      <c r="J185" s="5"/>
+      <c r="I185" s="4">
+        <v>298</v>
+      </c>
+      <c r="J185" s="5" t="s">
+        <v>260</v>
+      </c>
       <c r="K185" s="5"/>
-      <c r="L185" s="7"/>
-      <c r="M185" s="7"/>
-      <c r="N185" s="7"/>
+      <c r="L185" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M185" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="N185" s="7" t="s">
+        <v>242</v>
+      </c>
       <c r="O185" s="2"/>
       <c r="P185" s="7"/>
       <c r="Q185" s="2"/>
@@ -11586,13 +12068,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="253" customHeight="1" ht="18">
       <c r="A253" s="49"/>
-      <c r="B253" s="7"/>
-      <c r="C253" s="80"/>
-      <c r="D253" s="80"/>
-      <c r="E253" s="7"/>
-      <c r="F253" s="80"/>
-      <c r="G253" s="80"/>
-      <c r="H253" s="80"/>
+      <c r="B253" s="2"/>
+      <c r="C253" s="3"/>
+      <c r="D253" s="3"/>
+      <c r="E253" s="2"/>
+      <c r="F253" s="3"/>
+      <c r="G253" s="3"/>
+      <c r="H253" s="3"/>
       <c r="I253" s="4"/>
       <c r="J253" s="5"/>
       <c r="K253" s="5"/>
@@ -12619,7 +13101,7 @@
       <c r="T299" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="300" customHeight="1" ht="18">
-      <c r="A300" s="49"/>
+      <c r="A300" s="7"/>
       <c r="B300" s="2"/>
       <c r="C300" s="3"/>
       <c r="D300" s="3"/>
@@ -15367,28 +15849,6 @@
       <c r="R424" s="2"/>
       <c r="S424" s="2"/>
       <c r="T424" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="425" customHeight="1" ht="18">
-      <c r="A425" s="7"/>
-      <c r="B425" s="2"/>
-      <c r="C425" s="3"/>
-      <c r="D425" s="3"/>
-      <c r="E425" s="2"/>
-      <c r="F425" s="3"/>
-      <c r="G425" s="3"/>
-      <c r="H425" s="3"/>
-      <c r="I425" s="4"/>
-      <c r="J425" s="5"/>
-      <c r="K425" s="5"/>
-      <c r="L425" s="7"/>
-      <c r="M425" s="7"/>
-      <c r="N425" s="7"/>
-      <c r="O425" s="2"/>
-      <c r="P425" s="7"/>
-      <c r="Q425" s="2"/>
-      <c r="R425" s="2"/>
-      <c r="S425" s="2"/>
-      <c r="T425" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="19">

</xml_diff>

<commit_message>
- polishing to remove comment newline and invisible unicode copied from publication text
</commit_message>
<xml_diff>
--- a/DuctilitySearch_Feb24.xlsx
+++ b/DuctilitySearch_Feb24.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1742" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1746" uniqueCount="262">
   <si>
     <t>Metadata</t>
   </si>
@@ -788,21 +788,24 @@
     <t>VAM+HF+H+CR+RX</t>
   </si>
   <si>
+    <t>Lamellar phases in FCC grains; ultrafine grain 0.43um; hot forged at 1,423K; homogenization in a vacuum at 1,373K for 2h; cold rolling for 90% reduction; recrystallization at 1,173K for 150s</t>
+  </si>
+  <si>
+    <t>tensile yield strength</t>
+  </si>
+  <si>
+    <t>2.08e9</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>10.1038/s41563-024-01871-7</t>
+  </si>
+  <si>
     <t>Lamellar phases in FCC grains; ultrafine grain 0.43um; hot forged at 1,423 K; homogenization in a vacuum at 1,373 K for 2 h; cold rolling for 90% reduction; recrystallization at 1,173 K for 150s</t>
   </si>
   <si>
-    <t>tensile yield strength</t>
-  </si>
-  <si>
-    <t>2.08e9</t>
-  </si>
-  <si>
-    <t>F2</t>
-  </si>
-  <si>
-    <t>10.1038/s41563-024-01871-7</t>
-  </si>
-  <si>
     <t>strain rate 0.5e-3; liquid nitrogen</t>
   </si>
   <si>
@@ -863,8 +866,7 @@
     <t>H</t>
   </si>
   <si>
-    <t>homogenized at 1100C for 10h; homogenization stabilizes the CrMoZr phase Fd-3m Cu2Mg-typed Laves phase
-; mid-button cut</t>
+    <t>homogenized at 1100C for 10h; homogenization stabilizes the CrMoZr phase Fd-3m Cu2Mg-typed Laves phase; mid-button cut</t>
   </si>
   <si>
     <t>1275e6</t>
@@ -1738,11 +1740,11 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2074,7 +2076,7 @@
     <col min="2" max="2" style="89" width="31.005" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="90" width="16.290714285714284" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="90" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="89" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="89" width="27.290714285714284" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="90" width="17.862142857142857" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="90" width="19.290714285714284" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="90" width="21.005" customWidth="1" bestFit="1"/>
@@ -9470,7 +9472,7 @@
         <v>226</v>
       </c>
       <c r="E162" s="6" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F162" s="3" t="s">
         <v>228</v>
@@ -9479,13 +9481,13 @@
         <v>29</v>
       </c>
       <c r="H162" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I162" s="4">
         <v>77</v>
       </c>
       <c r="J162" s="5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="K162" s="5"/>
       <c r="L162" s="6" t="s">
@@ -9518,7 +9520,7 @@
         <v>226</v>
       </c>
       <c r="E163" s="6" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F163" s="3" t="s">
         <v>228</v>
@@ -9527,13 +9529,13 @@
         <v>29</v>
       </c>
       <c r="H163" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="I163" s="4">
         <v>4</v>
       </c>
       <c r="J163" s="5" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="K163" s="5"/>
       <c r="L163" s="6" t="s">
@@ -9566,10 +9568,10 @@
         <v>226</v>
       </c>
       <c r="E164" s="6" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F164" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G164" s="3" t="s">
         <v>29</v>
@@ -9581,7 +9583,7 @@
         <v>298</v>
       </c>
       <c r="J164" s="5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="K164" s="5"/>
       <c r="L164" s="6" t="s">
@@ -9614,22 +9616,22 @@
         <v>226</v>
       </c>
       <c r="E165" s="6" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G165" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H165" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I165" s="4">
         <v>77</v>
       </c>
       <c r="J165" s="5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="K165" s="5"/>
       <c r="L165" s="6" t="s">
@@ -9662,22 +9664,22 @@
         <v>226</v>
       </c>
       <c r="E166" s="6" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F166" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G166" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H166" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="I166" s="4">
         <v>4</v>
       </c>
       <c r="J166" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="K166" s="5"/>
       <c r="L166" s="6" t="s">
@@ -9710,7 +9712,7 @@
         <v>226</v>
       </c>
       <c r="E167" s="6" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F167" s="3" t="s">
         <v>79</v>
@@ -9758,7 +9760,7 @@
         <v>226</v>
       </c>
       <c r="E168" s="6" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F168" s="3" t="s">
         <v>79</v>
@@ -9767,7 +9769,7 @@
         <v>29</v>
       </c>
       <c r="H168" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I168" s="4">
         <v>77</v>
@@ -9806,7 +9808,7 @@
         <v>226</v>
       </c>
       <c r="E169" s="6" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F169" s="3" t="s">
         <v>79</v>
@@ -9815,7 +9817,7 @@
         <v>29</v>
       </c>
       <c r="H169" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="I169" s="4">
         <v>4</v>
@@ -9845,7 +9847,7 @@
         <v>10</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C170" s="80" t="s">
         <v>65</v>
@@ -9854,7 +9856,7 @@
         <v>66</v>
       </c>
       <c r="E170" s="7" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F170" s="80" t="s">
         <v>107</v>
@@ -9876,10 +9878,10 @@
         <v>80</v>
       </c>
       <c r="M170" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N170" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O170" s="2"/>
       <c r="P170" s="7"/>
@@ -9893,7 +9895,7 @@
         <v>10</v>
       </c>
       <c r="B171" s="7" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C171" s="80" t="s">
         <v>65</v>
@@ -9902,7 +9904,7 @@
         <v>66</v>
       </c>
       <c r="E171" s="7" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F171" s="80" t="s">
         <v>107</v>
@@ -9924,10 +9926,10 @@
         <v>80</v>
       </c>
       <c r="M171" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N171" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O171" s="2"/>
       <c r="P171" s="7"/>
@@ -9941,7 +9943,7 @@
         <v>10</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C172" s="80" t="s">
         <v>65</v>
@@ -9950,13 +9952,13 @@
         <v>66</v>
       </c>
       <c r="E172" s="7" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F172" s="85" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="G172" s="85" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H172" s="80"/>
       <c r="I172" s="4"/>
@@ -9964,10 +9966,10 @@
       <c r="K172" s="5"/>
       <c r="L172" s="7"/>
       <c r="M172" s="7" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="N172" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O172" s="2"/>
       <c r="P172" s="7"/>
@@ -9981,16 +9983,16 @@
         <v>10</v>
       </c>
       <c r="B173" s="7" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C173" s="80" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D173" s="80" t="s">
         <v>66</v>
       </c>
       <c r="E173" s="7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F173" s="80" t="s">
         <v>107</v>
@@ -10012,10 +10014,10 @@
         <v>80</v>
       </c>
       <c r="M173" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N173" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O173" s="2"/>
       <c r="P173" s="7"/>
@@ -10029,16 +10031,16 @@
         <v>10</v>
       </c>
       <c r="B174" s="7" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C174" s="80" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D174" s="80" t="s">
         <v>66</v>
       </c>
       <c r="E174" s="7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F174" s="80" t="s">
         <v>107</v>
@@ -10060,10 +10062,10 @@
         <v>80</v>
       </c>
       <c r="M174" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N174" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O174" s="2"/>
       <c r="P174" s="7"/>
@@ -10072,21 +10074,21 @@
       <c r="S174" s="2"/>
       <c r="T174" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75">
       <c r="A175" s="49">
         <v>10</v>
       </c>
       <c r="B175" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C175" s="80" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D175" s="80" t="s">
-        <v>251</v>
-      </c>
-      <c r="E175" s="7" t="s">
         <v>252</v>
+      </c>
+      <c r="E175" s="86" t="s">
+        <v>253</v>
       </c>
       <c r="F175" s="80" t="s">
         <v>107</v>
@@ -10108,10 +10110,10 @@
         <v>80</v>
       </c>
       <c r="M175" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N175" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O175" s="2"/>
       <c r="P175" s="7"/>
@@ -10125,18 +10127,18 @@
         <v>10</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="C176" s="86" t="s">
+        <v>240</v>
+      </c>
+      <c r="C176" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="D176" s="86" t="s">
+      <c r="D176" s="87" t="s">
         <v>66</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="F176" s="86" t="s">
+        <v>241</v>
+      </c>
+      <c r="F176" s="87" t="s">
         <v>88</v>
       </c>
       <c r="G176" s="80" t="s">
@@ -10147,19 +10149,19 @@
         <v>298</v>
       </c>
       <c r="J176" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="K176" s="5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="L176" s="7" t="s">
         <v>33</v>
       </c>
       <c r="M176" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N176" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O176" s="2"/>
       <c r="P176" s="7"/>
@@ -10173,18 +10175,18 @@
         <v>10</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="C177" s="86" t="s">
+        <v>244</v>
+      </c>
+      <c r="C177" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="D177" s="86" t="s">
+      <c r="D177" s="87" t="s">
         <v>66</v>
       </c>
       <c r="E177" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="F177" s="86" t="s">
+        <v>241</v>
+      </c>
+      <c r="F177" s="87" t="s">
         <v>88</v>
       </c>
       <c r="G177" s="80" t="s">
@@ -10195,19 +10197,19 @@
         <v>298</v>
       </c>
       <c r="J177" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="K177" s="5" t="s">
         <v>255</v>
-      </c>
-      <c r="K177" s="5" t="s">
-        <v>254</v>
       </c>
       <c r="L177" s="7" t="s">
         <v>33</v>
       </c>
       <c r="M177" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N177" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O177" s="2"/>
       <c r="P177" s="7"/>
@@ -10221,18 +10223,18 @@
         <v>10</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="C178" s="86" t="s">
         <v>248</v>
       </c>
-      <c r="D178" s="86" t="s">
+      <c r="C178" s="87" t="s">
+        <v>249</v>
+      </c>
+      <c r="D178" s="87" t="s">
         <v>66</v>
       </c>
       <c r="E178" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="F178" s="86" t="s">
+        <v>250</v>
+      </c>
+      <c r="F178" s="87" t="s">
         <v>88</v>
       </c>
       <c r="G178" s="80" t="s">
@@ -10243,19 +10245,19 @@
         <v>298</v>
       </c>
       <c r="J178" s="5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="K178" s="5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="L178" s="7" t="s">
         <v>33</v>
       </c>
       <c r="M178" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N178" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O178" s="2"/>
       <c r="P178" s="7"/>
@@ -10269,18 +10271,18 @@
         <v>10</v>
       </c>
       <c r="B179" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C179" s="87" t="s">
+        <v>249</v>
+      </c>
+      <c r="D179" s="87" t="s">
+        <v>66</v>
+      </c>
+      <c r="E179" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="C179" s="86" t="s">
-        <v>248</v>
-      </c>
-      <c r="D179" s="86" t="s">
-        <v>66</v>
-      </c>
-      <c r="E179" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="F179" s="86" t="s">
+      <c r="F179" s="87" t="s">
         <v>88</v>
       </c>
       <c r="G179" s="80" t="s">
@@ -10291,19 +10293,19 @@
         <v>298</v>
       </c>
       <c r="J179" s="5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="K179" s="5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="L179" s="7" t="s">
         <v>33</v>
       </c>
       <c r="M179" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N179" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O179" s="2"/>
       <c r="P179" s="7"/>
@@ -10317,18 +10319,18 @@
         <v>10</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C180" s="86" t="s">
-        <v>248</v>
-      </c>
-      <c r="D180" s="86" t="s">
-        <v>251</v>
-      </c>
-      <c r="E180" s="87" t="s">
+        <v>245</v>
+      </c>
+      <c r="C180" s="87" t="s">
+        <v>249</v>
+      </c>
+      <c r="D180" s="87" t="s">
         <v>252</v>
       </c>
-      <c r="F180" s="86" t="s">
+      <c r="E180" s="86" t="s">
+        <v>253</v>
+      </c>
+      <c r="F180" s="87" t="s">
         <v>88</v>
       </c>
       <c r="G180" s="80" t="s">
@@ -10339,19 +10341,19 @@
         <v>298</v>
       </c>
       <c r="J180" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="K180" s="5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="L180" s="7" t="s">
         <v>33</v>
       </c>
       <c r="M180" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N180" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O180" s="2"/>
       <c r="P180" s="7"/>
@@ -10365,18 +10367,18 @@
         <v>10</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="C181" s="86" t="s">
+        <v>240</v>
+      </c>
+      <c r="C181" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="D181" s="86" t="s">
+      <c r="D181" s="87" t="s">
         <v>66</v>
       </c>
       <c r="E181" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="F181" s="86" t="s">
+        <v>241</v>
+      </c>
+      <c r="F181" s="87" t="s">
         <v>149</v>
       </c>
       <c r="G181" s="80" t="s">
@@ -10387,7 +10389,7 @@
         <v>298</v>
       </c>
       <c r="J181" s="5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="K181" s="5" t="s">
         <v>32</v>
@@ -10396,10 +10398,10 @@
         <v>33</v>
       </c>
       <c r="M181" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N181" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O181" s="2"/>
       <c r="P181" s="7"/>
@@ -10413,18 +10415,18 @@
         <v>10</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="C182" s="86" t="s">
+        <v>244</v>
+      </c>
+      <c r="C182" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="D182" s="86" t="s">
+      <c r="D182" s="87" t="s">
         <v>66</v>
       </c>
       <c r="E182" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="F182" s="86" t="s">
+        <v>241</v>
+      </c>
+      <c r="F182" s="87" t="s">
         <v>149</v>
       </c>
       <c r="G182" s="80" t="s">
@@ -10437,15 +10439,17 @@
       <c r="J182" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="K182" s="5"/>
+      <c r="K182" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="L182" s="7" t="s">
         <v>33</v>
       </c>
       <c r="M182" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N182" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O182" s="2"/>
       <c r="P182" s="7"/>
@@ -10459,18 +10463,18 @@
         <v>10</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="C183" s="86" t="s">
         <v>248</v>
       </c>
-      <c r="D183" s="86" t="s">
+      <c r="C183" s="87" t="s">
+        <v>249</v>
+      </c>
+      <c r="D183" s="87" t="s">
         <v>66</v>
       </c>
       <c r="E183" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="F183" s="86" t="s">
+        <v>250</v>
+      </c>
+      <c r="F183" s="87" t="s">
         <v>149</v>
       </c>
       <c r="G183" s="80" t="s">
@@ -10481,17 +10485,19 @@
         <v>298</v>
       </c>
       <c r="J183" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="K183" s="5"/>
+        <v>260</v>
+      </c>
+      <c r="K183" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="L183" s="7" t="s">
         <v>33</v>
       </c>
       <c r="M183" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N183" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O183" s="2"/>
       <c r="P183" s="7"/>
@@ -10505,18 +10511,18 @@
         <v>10</v>
       </c>
       <c r="B184" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C184" s="87" t="s">
+        <v>249</v>
+      </c>
+      <c r="D184" s="87" t="s">
+        <v>66</v>
+      </c>
+      <c r="E184" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="C184" s="86" t="s">
-        <v>248</v>
-      </c>
-      <c r="D184" s="86" t="s">
-        <v>66</v>
-      </c>
-      <c r="E184" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="F184" s="86" t="s">
+      <c r="F184" s="87" t="s">
         <v>149</v>
       </c>
       <c r="G184" s="80" t="s">
@@ -10529,15 +10535,17 @@
       <c r="J184" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="K184" s="5"/>
+      <c r="K184" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="L184" s="7" t="s">
         <v>33</v>
       </c>
       <c r="M184" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N184" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O184" s="2"/>
       <c r="P184" s="7"/>
@@ -10546,23 +10554,23 @@
       <c r="S184" s="2"/>
       <c r="T184" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="19.5">
       <c r="A185" s="49">
         <v>10</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C185" s="86" t="s">
-        <v>248</v>
-      </c>
-      <c r="D185" s="86" t="s">
-        <v>251</v>
-      </c>
-      <c r="E185" s="87" t="s">
+        <v>245</v>
+      </c>
+      <c r="C185" s="87" t="s">
+        <v>249</v>
+      </c>
+      <c r="D185" s="87" t="s">
         <v>252</v>
       </c>
-      <c r="F185" s="86" t="s">
+      <c r="E185" s="86" t="s">
+        <v>253</v>
+      </c>
+      <c r="F185" s="87" t="s">
         <v>149</v>
       </c>
       <c r="G185" s="80" t="s">
@@ -10573,17 +10581,19 @@
         <v>298</v>
       </c>
       <c r="J185" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="K185" s="5"/>
+        <v>261</v>
+      </c>
+      <c r="K185" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="L185" s="7" t="s">
         <v>33</v>
       </c>
       <c r="M185" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N185" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O185" s="2"/>
       <c r="P185" s="7"/>

</xml_diff>

<commit_message>
- polishing to remove invisible unicode copied from publication text
</commit_message>
<xml_diff>
--- a/DuctilitySearch_Feb24.xlsx
+++ b/DuctilitySearch_Feb24.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1746" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1744" uniqueCount="260">
   <si>
     <t>Metadata</t>
   </si>
@@ -803,9 +803,6 @@
     <t>10.1038/s41563-024-01871-7</t>
   </si>
   <si>
-    <t>Lamellar phases in FCC grains; ultrafine grain 0.43um; hot forged at 1,423 K; homogenization in a vacuum at 1,373 K for 2 h; cold rolling for 90% reduction; recrystallization at 1,173 K for 150s</t>
-  </si>
-  <si>
     <t>strain rate 0.5e-3; liquid nitrogen</t>
   </si>
   <si>
@@ -843,9 +840,6 @@
   </si>
   <si>
     <t>Hf0.5 Mo0.5 Nb Ti Zr Cr0.3</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>S3</t>
@@ -1483,7 +1477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="93">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1737,13 +1731,10 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -2072,26 +2063,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="88" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="89" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="90" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="90" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="89" width="27.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="90" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="90" width="19.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="90" width="21.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="91" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="92" width="25.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="92" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="93" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="93" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="93" width="34.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="89" width="39.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="88" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="89" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="89" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="89" width="17.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="89" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="87" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="88" width="31.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="89" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="89" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="88" width="27.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="89" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="89" width="19.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="89" width="21.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="90" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="91" width="25.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="91" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="92" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="92" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="92" width="34.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="88" width="39.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="87" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="88" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="88" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="88" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="88" width="17.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
@@ -9448,7 +9439,7 @@
       <c r="M161" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="N161" s="7" t="s">
+      <c r="N161" s="6" t="s">
         <v>231</v>
       </c>
       <c r="O161" s="2"/>
@@ -9472,7 +9463,7 @@
         <v>226</v>
       </c>
       <c r="E162" s="6" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F162" s="3" t="s">
         <v>228</v>
@@ -9481,13 +9472,13 @@
         <v>29</v>
       </c>
       <c r="H162" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I162" s="4">
         <v>77</v>
       </c>
       <c r="J162" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K162" s="5"/>
       <c r="L162" s="6" t="s">
@@ -9496,7 +9487,7 @@
       <c r="M162" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="N162" s="7" t="s">
+      <c r="N162" s="6" t="s">
         <v>231</v>
       </c>
       <c r="O162" s="2"/>
@@ -9520,7 +9511,7 @@
         <v>226</v>
       </c>
       <c r="E163" s="6" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F163" s="3" t="s">
         <v>228</v>
@@ -9529,13 +9520,13 @@
         <v>29</v>
       </c>
       <c r="H163" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I163" s="4">
         <v>4</v>
       </c>
       <c r="J163" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K163" s="5"/>
       <c r="L163" s="6" t="s">
@@ -9544,7 +9535,7 @@
       <c r="M163" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="N163" s="7" t="s">
+      <c r="N163" s="6" t="s">
         <v>231</v>
       </c>
       <c r="O163" s="2"/>
@@ -9568,10 +9559,10 @@
         <v>226</v>
       </c>
       <c r="E164" s="6" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F164" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G164" s="3" t="s">
         <v>29</v>
@@ -9583,7 +9574,7 @@
         <v>298</v>
       </c>
       <c r="J164" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K164" s="5"/>
       <c r="L164" s="6" t="s">
@@ -9592,7 +9583,7 @@
       <c r="M164" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="N164" s="7" t="s">
+      <c r="N164" s="6" t="s">
         <v>231</v>
       </c>
       <c r="O164" s="2"/>
@@ -9616,22 +9607,22 @@
         <v>226</v>
       </c>
       <c r="E165" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="F165" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="G165" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H165" s="3" t="s">
         <v>232</v>
-      </c>
-      <c r="F165" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="G165" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H165" s="3" t="s">
-        <v>233</v>
       </c>
       <c r="I165" s="4">
         <v>77</v>
       </c>
       <c r="J165" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K165" s="5"/>
       <c r="L165" s="6" t="s">
@@ -9640,7 +9631,7 @@
       <c r="M165" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="N165" s="7" t="s">
+      <c r="N165" s="6" t="s">
         <v>231</v>
       </c>
       <c r="O165" s="2"/>
@@ -9664,22 +9655,22 @@
         <v>226</v>
       </c>
       <c r="E166" s="6" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F166" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G166" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H166" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I166" s="4">
         <v>4</v>
       </c>
       <c r="J166" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K166" s="5"/>
       <c r="L166" s="6" t="s">
@@ -9688,7 +9679,7 @@
       <c r="M166" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="N166" s="7" t="s">
+      <c r="N166" s="6" t="s">
         <v>231</v>
       </c>
       <c r="O166" s="2"/>
@@ -9712,7 +9703,7 @@
         <v>226</v>
       </c>
       <c r="E167" s="6" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F167" s="3" t="s">
         <v>79</v>
@@ -9736,7 +9727,7 @@
       <c r="M167" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="N167" s="7" t="s">
+      <c r="N167" s="6" t="s">
         <v>231</v>
       </c>
       <c r="O167" s="2"/>
@@ -9760,7 +9751,7 @@
         <v>226</v>
       </c>
       <c r="E168" s="6" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F168" s="3" t="s">
         <v>79</v>
@@ -9769,7 +9760,7 @@
         <v>29</v>
       </c>
       <c r="H168" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I168" s="4">
         <v>77</v>
@@ -9784,7 +9775,7 @@
       <c r="M168" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="N168" s="7" t="s">
+      <c r="N168" s="6" t="s">
         <v>231</v>
       </c>
       <c r="O168" s="2"/>
@@ -9808,7 +9799,7 @@
         <v>226</v>
       </c>
       <c r="E169" s="6" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F169" s="3" t="s">
         <v>79</v>
@@ -9817,7 +9808,7 @@
         <v>29</v>
       </c>
       <c r="H169" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I169" s="4">
         <v>4</v>
@@ -9832,7 +9823,7 @@
       <c r="M169" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="N169" s="7" t="s">
+      <c r="N169" s="6" t="s">
         <v>231</v>
       </c>
       <c r="O169" s="2"/>
@@ -9846,22 +9837,22 @@
       <c r="A170" s="49">
         <v>10</v>
       </c>
-      <c r="B170" s="7" t="s">
+      <c r="B170" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E170" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="C170" s="80" t="s">
-        <v>65</v>
-      </c>
-      <c r="D170" s="80" t="s">
-        <v>66</v>
-      </c>
-      <c r="E170" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="F170" s="80" t="s">
+      <c r="F170" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G170" s="80" t="s">
+      <c r="G170" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H170" s="80"/>
@@ -9874,14 +9865,14 @@
       <c r="K170" s="5">
         <v>0.5</v>
       </c>
-      <c r="L170" s="7" t="s">
+      <c r="L170" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M170" s="7" t="s">
+      <c r="M170" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="N170" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="N170" s="7" t="s">
-        <v>243</v>
       </c>
       <c r="O170" s="2"/>
       <c r="P170" s="7"/>
@@ -9894,22 +9885,22 @@
       <c r="A171" s="49">
         <v>10</v>
       </c>
-      <c r="B171" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="C171" s="80" t="s">
+      <c r="B171" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="C171" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D171" s="80" t="s">
+      <c r="D171" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E171" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="F171" s="80" t="s">
+      <c r="E171" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="F171" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G171" s="80" t="s">
+      <c r="G171" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H171" s="80"/>
@@ -9922,14 +9913,14 @@
       <c r="K171" s="5">
         <v>0.5</v>
       </c>
-      <c r="L171" s="7" t="s">
+      <c r="L171" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M171" s="7" t="s">
+      <c r="M171" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="N171" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="N171" s="7" t="s">
-        <v>243</v>
       </c>
       <c r="O171" s="2"/>
       <c r="P171" s="7"/>
@@ -9942,34 +9933,30 @@
       <c r="A172" s="49">
         <v>10</v>
       </c>
-      <c r="B172" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C172" s="80" t="s">
+      <c r="B172" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="C172" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D172" s="80" t="s">
+      <c r="D172" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E172" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="F172" s="85" t="s">
-        <v>246</v>
-      </c>
-      <c r="G172" s="85" t="s">
-        <v>246</v>
-      </c>
+      <c r="E172" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="F172" s="3"/>
+      <c r="G172" s="3"/>
       <c r="H172" s="80"/>
       <c r="I172" s="4"/>
       <c r="J172" s="5"/>
       <c r="K172" s="5"/>
       <c r="L172" s="7"/>
-      <c r="M172" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="N172" s="7" t="s">
-        <v>243</v>
+      <c r="M172" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="N172" s="6" t="s">
+        <v>242</v>
       </c>
       <c r="O172" s="2"/>
       <c r="P172" s="7"/>
@@ -9982,22 +9969,22 @@
       <c r="A173" s="49">
         <v>10</v>
       </c>
-      <c r="B173" s="7" t="s">
+      <c r="B173" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="D173" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E173" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="C173" s="80" t="s">
-        <v>249</v>
-      </c>
-      <c r="D173" s="80" t="s">
-        <v>66</v>
-      </c>
-      <c r="E173" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="F173" s="80" t="s">
+      <c r="F173" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G173" s="80" t="s">
+      <c r="G173" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H173" s="80"/>
@@ -10010,14 +9997,14 @@
       <c r="K173" s="5">
         <v>0.5</v>
       </c>
-      <c r="L173" s="7" t="s">
+      <c r="L173" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M173" s="7" t="s">
+      <c r="M173" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="N173" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="N173" s="7" t="s">
-        <v>243</v>
       </c>
       <c r="O173" s="2"/>
       <c r="P173" s="7"/>
@@ -10030,22 +10017,22 @@
       <c r="A174" s="49">
         <v>10</v>
       </c>
-      <c r="B174" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="C174" s="80" t="s">
+      <c r="B174" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="D174" s="80" t="s">
+      <c r="C174" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="D174" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E174" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="F174" s="80" t="s">
+      <c r="E174" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="F174" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G174" s="80" t="s">
+      <c r="G174" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H174" s="80"/>
@@ -10058,14 +10045,14 @@
       <c r="K174" s="5">
         <v>0.5</v>
       </c>
-      <c r="L174" s="7" t="s">
+      <c r="L174" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M174" s="7" t="s">
+      <c r="M174" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="N174" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="N174" s="7" t="s">
-        <v>243</v>
       </c>
       <c r="O174" s="2"/>
       <c r="P174" s="7"/>
@@ -10078,22 +10065,22 @@
       <c r="A175" s="49">
         <v>10</v>
       </c>
-      <c r="B175" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C175" s="80" t="s">
-        <v>249</v>
-      </c>
-      <c r="D175" s="80" t="s">
-        <v>252</v>
-      </c>
-      <c r="E175" s="86" t="s">
-        <v>253</v>
-      </c>
-      <c r="F175" s="80" t="s">
+      <c r="B175" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="E175" s="85" t="s">
+        <v>251</v>
+      </c>
+      <c r="F175" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G175" s="80" t="s">
+      <c r="G175" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H175" s="80"/>
@@ -10106,14 +10093,14 @@
       <c r="K175" s="5">
         <v>0.5</v>
       </c>
-      <c r="L175" s="7" t="s">
+      <c r="L175" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M175" s="7" t="s">
+      <c r="M175" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="N175" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="N175" s="7" t="s">
-        <v>243</v>
       </c>
       <c r="O175" s="2"/>
       <c r="P175" s="7"/>
@@ -10127,21 +10114,21 @@
         <v>10</v>
       </c>
       <c r="B176" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C176" s="86" t="s">
+        <v>65</v>
+      </c>
+      <c r="D176" s="86" t="s">
+        <v>66</v>
+      </c>
+      <c r="E176" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="C176" s="87" t="s">
-        <v>65</v>
-      </c>
-      <c r="D176" s="87" t="s">
-        <v>66</v>
-      </c>
-      <c r="E176" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="F176" s="87" t="s">
+      <c r="F176" s="86" t="s">
         <v>88</v>
       </c>
-      <c r="G176" s="80" t="s">
+      <c r="G176" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H176" s="80"/>
@@ -10149,19 +10136,19 @@
         <v>298</v>
       </c>
       <c r="J176" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="K176" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="L176" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="L176" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M176" s="7" t="s">
+      <c r="M176" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="N176" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="N176" s="7" t="s">
-        <v>243</v>
       </c>
       <c r="O176" s="2"/>
       <c r="P176" s="7"/>
@@ -10175,21 +10162,21 @@
         <v>10</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C177" s="87" t="s">
+        <v>243</v>
+      </c>
+      <c r="C177" s="86" t="s">
         <v>65</v>
       </c>
-      <c r="D177" s="87" t="s">
+      <c r="D177" s="86" t="s">
         <v>66</v>
       </c>
       <c r="E177" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="F177" s="87" t="s">
+        <v>240</v>
+      </c>
+      <c r="F177" s="86" t="s">
         <v>88</v>
       </c>
-      <c r="G177" s="80" t="s">
+      <c r="G177" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H177" s="80"/>
@@ -10197,19 +10184,19 @@
         <v>298</v>
       </c>
       <c r="J177" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="K177" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="L177" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="L177" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M177" s="7" t="s">
+      <c r="M177" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="N177" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="N177" s="7" t="s">
-        <v>243</v>
       </c>
       <c r="O177" s="2"/>
       <c r="P177" s="7"/>
@@ -10223,21 +10210,21 @@
         <v>10</v>
       </c>
       <c r="B178" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C178" s="86" t="s">
+        <v>247</v>
+      </c>
+      <c r="D178" s="86" t="s">
+        <v>66</v>
+      </c>
+      <c r="E178" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="C178" s="87" t="s">
-        <v>249</v>
-      </c>
-      <c r="D178" s="87" t="s">
-        <v>66</v>
-      </c>
-      <c r="E178" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="F178" s="87" t="s">
+      <c r="F178" s="86" t="s">
         <v>88</v>
       </c>
-      <c r="G178" s="80" t="s">
+      <c r="G178" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H178" s="80"/>
@@ -10245,19 +10232,19 @@
         <v>298</v>
       </c>
       <c r="J178" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K178" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="L178" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="L178" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M178" s="7" t="s">
+      <c r="M178" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="N178" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="N178" s="7" t="s">
-        <v>243</v>
       </c>
       <c r="O178" s="2"/>
       <c r="P178" s="7"/>
@@ -10271,21 +10258,21 @@
         <v>10</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="C179" s="87" t="s">
         <v>249</v>
       </c>
-      <c r="D179" s="87" t="s">
+      <c r="C179" s="86" t="s">
+        <v>247</v>
+      </c>
+      <c r="D179" s="86" t="s">
         <v>66</v>
       </c>
       <c r="E179" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="F179" s="87" t="s">
+        <v>248</v>
+      </c>
+      <c r="F179" s="86" t="s">
         <v>88</v>
       </c>
-      <c r="G179" s="80" t="s">
+      <c r="G179" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H179" s="80"/>
@@ -10293,19 +10280,19 @@
         <v>298</v>
       </c>
       <c r="J179" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="K179" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="L179" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="L179" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M179" s="7" t="s">
+      <c r="M179" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="N179" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="N179" s="7" t="s">
-        <v>243</v>
       </c>
       <c r="O179" s="2"/>
       <c r="P179" s="7"/>
@@ -10319,21 +10306,21 @@
         <v>10</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="C180" s="87" t="s">
-        <v>249</v>
-      </c>
-      <c r="D180" s="87" t="s">
-        <v>252</v>
-      </c>
-      <c r="E180" s="86" t="s">
-        <v>253</v>
-      </c>
-      <c r="F180" s="87" t="s">
+        <v>244</v>
+      </c>
+      <c r="C180" s="86" t="s">
+        <v>247</v>
+      </c>
+      <c r="D180" s="86" t="s">
+        <v>250</v>
+      </c>
+      <c r="E180" s="85" t="s">
+        <v>251</v>
+      </c>
+      <c r="F180" s="86" t="s">
         <v>88</v>
       </c>
-      <c r="G180" s="80" t="s">
+      <c r="G180" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H180" s="80"/>
@@ -10341,19 +10328,19 @@
         <v>298</v>
       </c>
       <c r="J180" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="K180" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="L180" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="L180" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M180" s="7" t="s">
+      <c r="M180" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="N180" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="N180" s="7" t="s">
-        <v>243</v>
       </c>
       <c r="O180" s="2"/>
       <c r="P180" s="7"/>
@@ -10367,21 +10354,21 @@
         <v>10</v>
       </c>
       <c r="B181" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C181" s="86" t="s">
+        <v>65</v>
+      </c>
+      <c r="D181" s="86" t="s">
+        <v>66</v>
+      </c>
+      <c r="E181" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="C181" s="87" t="s">
-        <v>65</v>
-      </c>
-      <c r="D181" s="87" t="s">
-        <v>66</v>
-      </c>
-      <c r="E181" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="F181" s="87" t="s">
+      <c r="F181" s="86" t="s">
         <v>149</v>
       </c>
-      <c r="G181" s="80" t="s">
+      <c r="G181" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H181" s="80"/>
@@ -10389,19 +10376,19 @@
         <v>298</v>
       </c>
       <c r="J181" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K181" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L181" s="7" t="s">
+      <c r="L181" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M181" s="7" t="s">
+      <c r="M181" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="N181" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="N181" s="7" t="s">
-        <v>243</v>
       </c>
       <c r="O181" s="2"/>
       <c r="P181" s="7"/>
@@ -10415,21 +10402,21 @@
         <v>10</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C182" s="87" t="s">
+        <v>243</v>
+      </c>
+      <c r="C182" s="86" t="s">
         <v>65</v>
       </c>
-      <c r="D182" s="87" t="s">
+      <c r="D182" s="86" t="s">
         <v>66</v>
       </c>
       <c r="E182" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="F182" s="87" t="s">
+        <v>240</v>
+      </c>
+      <c r="F182" s="86" t="s">
         <v>149</v>
       </c>
-      <c r="G182" s="80" t="s">
+      <c r="G182" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H182" s="80"/>
@@ -10442,14 +10429,14 @@
       <c r="K182" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L182" s="7" t="s">
+      <c r="L182" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M182" s="7" t="s">
+      <c r="M182" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="N182" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="N182" s="7" t="s">
-        <v>243</v>
       </c>
       <c r="O182" s="2"/>
       <c r="P182" s="7"/>
@@ -10463,21 +10450,21 @@
         <v>10</v>
       </c>
       <c r="B183" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C183" s="86" t="s">
+        <v>247</v>
+      </c>
+      <c r="D183" s="86" t="s">
+        <v>66</v>
+      </c>
+      <c r="E183" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="C183" s="87" t="s">
-        <v>249</v>
-      </c>
-      <c r="D183" s="87" t="s">
-        <v>66</v>
-      </c>
-      <c r="E183" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="F183" s="87" t="s">
+      <c r="F183" s="86" t="s">
         <v>149</v>
       </c>
-      <c r="G183" s="80" t="s">
+      <c r="G183" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H183" s="80"/>
@@ -10485,19 +10472,19 @@
         <v>298</v>
       </c>
       <c r="J183" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="K183" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L183" s="7" t="s">
+      <c r="L183" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M183" s="7" t="s">
+      <c r="M183" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="N183" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="N183" s="7" t="s">
-        <v>243</v>
       </c>
       <c r="O183" s="2"/>
       <c r="P183" s="7"/>
@@ -10511,21 +10498,21 @@
         <v>10</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="C184" s="87" t="s">
         <v>249</v>
       </c>
-      <c r="D184" s="87" t="s">
+      <c r="C184" s="86" t="s">
+        <v>247</v>
+      </c>
+      <c r="D184" s="86" t="s">
         <v>66</v>
       </c>
       <c r="E184" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="F184" s="87" t="s">
+        <v>248</v>
+      </c>
+      <c r="F184" s="86" t="s">
         <v>149</v>
       </c>
-      <c r="G184" s="80" t="s">
+      <c r="G184" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H184" s="80"/>
@@ -10538,14 +10525,14 @@
       <c r="K184" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L184" s="7" t="s">
+      <c r="L184" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M184" s="7" t="s">
+      <c r="M184" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="N184" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="N184" s="7" t="s">
-        <v>243</v>
       </c>
       <c r="O184" s="2"/>
       <c r="P184" s="7"/>
@@ -10559,21 +10546,21 @@
         <v>10</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="C185" s="87" t="s">
-        <v>249</v>
-      </c>
-      <c r="D185" s="87" t="s">
-        <v>252</v>
-      </c>
-      <c r="E185" s="86" t="s">
-        <v>253</v>
-      </c>
-      <c r="F185" s="87" t="s">
+        <v>244</v>
+      </c>
+      <c r="C185" s="86" t="s">
+        <v>247</v>
+      </c>
+      <c r="D185" s="86" t="s">
+        <v>250</v>
+      </c>
+      <c r="E185" s="85" t="s">
+        <v>251</v>
+      </c>
+      <c r="F185" s="86" t="s">
         <v>149</v>
       </c>
-      <c r="G185" s="80" t="s">
+      <c r="G185" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H185" s="80"/>
@@ -10581,19 +10568,19 @@
         <v>298</v>
       </c>
       <c r="J185" s="5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="K185" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L185" s="7" t="s">
+      <c r="L185" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M185" s="7" t="s">
+      <c r="M185" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="N185" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="N185" s="7" t="s">
-        <v>243</v>
       </c>
       <c r="O185" s="2"/>
       <c r="P185" s="7"/>

</xml_diff>

<commit_message>
- saving error fix
</commit_message>
<xml_diff>
--- a/DuctilitySearch_Feb24.xlsx
+++ b/DuctilitySearch_Feb24.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2298" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2333" uniqueCount="323">
   <si>
     <t>Metadata</t>
   </si>
@@ -906,9 +906,6 @@
   </si>
   <si>
     <t>W Mo V Cr Ta</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>ceramic ball milling before VAM</t>
@@ -1663,7 +1660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="92">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1919,9 +1916,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2249,26 +2243,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="87" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="88" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="89" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="89" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="88" width="27.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="89" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="89" width="19.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="89" width="21.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="90" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="91" width="25.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="91" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="92" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="92" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="92" width="34.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="88" width="39.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="87" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="88" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="88" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="88" width="17.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="88" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="86" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="87" width="31.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="88" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="88" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="87" width="27.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="88" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="88" width="19.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="88" width="21.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="89" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="90" width="25.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="90" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="91" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="91" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="91" width="34.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="87" width="39.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="86" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="87" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="87" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="87" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="87" width="17.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
@@ -10247,7 +10241,7 @@
       <c r="S174" s="2"/>
       <c r="T174" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="69.75">
       <c r="A175" s="49">
         <v>10</v>
       </c>
@@ -10487,7 +10481,7 @@
       <c r="S179" s="2"/>
       <c r="T179" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="69.75">
       <c r="A180" s="49">
         <v>10</v>
       </c>
@@ -10679,7 +10673,7 @@
       <c r="S183" s="2"/>
       <c r="T183" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="18.75">
       <c r="A184" s="49">
         <v>10</v>
       </c>
@@ -10727,7 +10721,7 @@
       <c r="S184" s="2"/>
       <c r="T184" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="69.75">
       <c r="A185" s="49">
         <v>10</v>
       </c>
@@ -10775,23 +10769,23 @@
       <c r="S185" s="2"/>
       <c r="T185" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="18.75">
       <c r="A186" s="49">
         <v>11</v>
       </c>
-      <c r="B186" s="7" t="s">
+      <c r="B186" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="C186" s="80" t="s">
+      <c r="C186" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D186" s="80" t="s">
+      <c r="D186" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E186" s="7" t="s">
+      <c r="E186" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="F186" s="80" t="s">
+      <c r="F186" s="3" t="s">
         <v>88</v>
       </c>
       <c r="G186" s="3" t="s">
@@ -10808,10 +10802,10 @@
       <c r="L186" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M186" s="7" t="s">
+      <c r="M186" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="N186" s="7" t="s">
+      <c r="N186" s="6" t="s">
         <v>265</v>
       </c>
       <c r="O186" s="2"/>
@@ -10821,23 +10815,21 @@
       <c r="S186" s="2"/>
       <c r="T186" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="18.75">
       <c r="A187" s="49">
         <v>11</v>
       </c>
-      <c r="B187" s="7" t="s">
+      <c r="B187" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="C187" s="86" t="s">
+      <c r="C187" s="3"/>
+      <c r="D187" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E187" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="D187" s="80" t="s">
-        <v>66</v>
-      </c>
-      <c r="E187" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="F187" s="80" t="s">
+      <c r="F187" s="3" t="s">
         <v>88</v>
       </c>
       <c r="G187" s="3" t="s">
@@ -10848,16 +10840,16 @@
         <v>298</v>
       </c>
       <c r="J187" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K187" s="5"/>
       <c r="L187" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M187" s="7" t="s">
+      <c r="M187" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="N187" s="7" t="s">
+      <c r="N187" s="6" t="s">
         <v>265</v>
       </c>
       <c r="O187" s="2"/>
@@ -10867,23 +10859,23 @@
       <c r="S187" s="2"/>
       <c r="T187" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="18.75">
       <c r="A188" s="49">
         <v>11</v>
       </c>
-      <c r="B188" s="7" t="s">
+      <c r="B188" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="C188" s="80" t="s">
+      <c r="C188" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D188" s="80" t="s">
+      <c r="D188" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E188" s="7" t="s">
+      <c r="E188" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="F188" s="80" t="s">
+      <c r="F188" s="3" t="s">
         <v>88</v>
       </c>
       <c r="G188" s="3" t="s">
@@ -10894,16 +10886,16 @@
         <v>1073</v>
       </c>
       <c r="J188" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K188" s="5"/>
       <c r="L188" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M188" s="7" t="s">
+      <c r="M188" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="N188" s="7" t="s">
+      <c r="N188" s="6" t="s">
         <v>265</v>
       </c>
       <c r="O188" s="2"/>
@@ -10913,23 +10905,23 @@
       <c r="S188" s="2"/>
       <c r="T188" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="18.75">
       <c r="A189" s="49">
         <v>11</v>
       </c>
-      <c r="B189" s="7" t="s">
+      <c r="B189" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="C189" s="80" t="s">
+      <c r="C189" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D189" s="80" t="s">
+      <c r="D189" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E189" s="7" t="s">
+      <c r="E189" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="F189" s="80" t="s">
+      <c r="F189" s="3" t="s">
         <v>88</v>
       </c>
       <c r="G189" s="3" t="s">
@@ -10940,16 +10932,16 @@
         <v>1273</v>
       </c>
       <c r="J189" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K189" s="5"/>
       <c r="L189" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M189" s="7" t="s">
+      <c r="M189" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="N189" s="7" t="s">
+      <c r="N189" s="6" t="s">
         <v>265</v>
       </c>
       <c r="O189" s="2"/>
@@ -10959,21 +10951,21 @@
       <c r="S189" s="2"/>
       <c r="T189" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="18.75">
       <c r="A190" s="49">
         <v>11</v>
       </c>
-      <c r="B190" s="7" t="s">
+      <c r="B190" s="6" t="s">
         <v>266</v>
       </c>
       <c r="C190" s="80"/>
-      <c r="D190" s="80" t="s">
+      <c r="D190" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E190" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="F190" s="80" t="s">
+      <c r="E190" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="F190" s="3" t="s">
         <v>88</v>
       </c>
       <c r="G190" s="3" t="s">
@@ -10984,16 +10976,16 @@
         <v>1273</v>
       </c>
       <c r="J190" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K190" s="5"/>
       <c r="L190" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M190" s="7" t="s">
+      <c r="M190" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="N190" s="7" t="s">
+      <c r="N190" s="6" t="s">
         <v>265</v>
       </c>
       <c r="O190" s="2"/>
@@ -11003,21 +10995,21 @@
       <c r="S190" s="2"/>
       <c r="T190" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="18.75">
       <c r="A191" s="49">
         <v>11</v>
       </c>
-      <c r="B191" s="7" t="s">
+      <c r="B191" s="6" t="s">
         <v>266</v>
       </c>
       <c r="C191" s="80"/>
-      <c r="D191" s="80" t="s">
+      <c r="D191" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E191" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="F191" s="80" t="s">
+      <c r="E191" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="F191" s="3" t="s">
         <v>88</v>
       </c>
       <c r="G191" s="3" t="s">
@@ -11028,16 +11020,16 @@
         <v>1473</v>
       </c>
       <c r="J191" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K191" s="5"/>
       <c r="L191" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M191" s="7" t="s">
+      <c r="M191" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="N191" s="7" t="s">
+      <c r="N191" s="6" t="s">
         <v>265</v>
       </c>
       <c r="O191" s="2"/>
@@ -11047,23 +11039,23 @@
       <c r="S191" s="2"/>
       <c r="T191" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="18.75">
       <c r="A192" s="49">
         <v>11</v>
       </c>
-      <c r="B192" s="7" t="s">
+      <c r="B192" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="C192" s="80" t="s">
+      <c r="C192" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D192" s="80" t="s">
+      <c r="D192" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E192" s="7" t="s">
+      <c r="E192" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="F192" s="80" t="s">
+      <c r="F192" s="3" t="s">
         <v>149</v>
       </c>
       <c r="G192" s="3" t="s">
@@ -11074,16 +11066,16 @@
         <v>298</v>
       </c>
       <c r="J192" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K192" s="5"/>
       <c r="L192" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M192" s="7" t="s">
+      <c r="M192" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="N192" s="7" t="s">
+      <c r="N192" s="6" t="s">
         <v>265</v>
       </c>
       <c r="O192" s="2"/>
@@ -11097,17 +11089,17 @@
       <c r="A193" s="49">
         <v>11</v>
       </c>
-      <c r="B193" s="7" t="s">
+      <c r="B193" s="6" t="s">
         <v>266</v>
       </c>
       <c r="C193" s="80"/>
-      <c r="D193" s="80" t="s">
+      <c r="D193" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E193" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="F193" s="80" t="s">
+      <c r="E193" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="F193" s="3" t="s">
         <v>149</v>
       </c>
       <c r="G193" s="3" t="s">
@@ -11118,16 +11110,16 @@
         <v>298</v>
       </c>
       <c r="J193" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K193" s="5"/>
       <c r="L193" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M193" s="7" t="s">
+      <c r="M193" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="N193" s="7" t="s">
+      <c r="N193" s="6" t="s">
         <v>265</v>
       </c>
       <c r="O193" s="2"/>
@@ -11141,19 +11133,19 @@
       <c r="A194" s="49">
         <v>11</v>
       </c>
-      <c r="B194" s="7" t="s">
+      <c r="B194" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="C194" s="80" t="s">
+      <c r="C194" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D194" s="80" t="s">
+      <c r="D194" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E194" s="7" t="s">
+      <c r="E194" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="F194" s="80" t="s">
+      <c r="F194" s="3" t="s">
         <v>149</v>
       </c>
       <c r="G194" s="3" t="s">
@@ -11164,16 +11156,16 @@
         <v>1073</v>
       </c>
       <c r="J194" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K194" s="5"/>
       <c r="L194" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M194" s="7" t="s">
+      <c r="M194" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="N194" s="7" t="s">
+      <c r="N194" s="6" t="s">
         <v>265</v>
       </c>
       <c r="O194" s="2"/>
@@ -11187,19 +11179,19 @@
       <c r="A195" s="49">
         <v>11</v>
       </c>
-      <c r="B195" s="7" t="s">
+      <c r="B195" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="C195" s="80" t="s">
+      <c r="C195" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D195" s="80" t="s">
+      <c r="D195" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E195" s="7" t="s">
+      <c r="E195" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="F195" s="80" t="s">
+      <c r="F195" s="3" t="s">
         <v>149</v>
       </c>
       <c r="G195" s="3" t="s">
@@ -11210,16 +11202,16 @@
         <v>1273</v>
       </c>
       <c r="J195" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="K195" s="5"/>
       <c r="L195" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M195" s="7" t="s">
+      <c r="M195" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="N195" s="7" t="s">
+      <c r="N195" s="6" t="s">
         <v>265</v>
       </c>
       <c r="O195" s="2"/>
@@ -11233,17 +11225,17 @@
       <c r="A196" s="49">
         <v>11</v>
       </c>
-      <c r="B196" s="7" t="s">
+      <c r="B196" s="6" t="s">
         <v>266</v>
       </c>
       <c r="C196" s="80"/>
-      <c r="D196" s="80" t="s">
+      <c r="D196" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E196" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="F196" s="80" t="s">
+      <c r="E196" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="F196" s="3" t="s">
         <v>149</v>
       </c>
       <c r="G196" s="3" t="s">
@@ -11254,16 +11246,16 @@
         <v>1273</v>
       </c>
       <c r="J196" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K196" s="5"/>
       <c r="L196" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M196" s="7" t="s">
+      <c r="M196" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="N196" s="7" t="s">
+      <c r="N196" s="6" t="s">
         <v>265</v>
       </c>
       <c r="O196" s="2"/>
@@ -11277,19 +11269,19 @@
       <c r="A197" s="49">
         <v>11</v>
       </c>
-      <c r="B197" s="7" t="s">
+      <c r="B197" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="C197" s="80" t="s">
+      <c r="C197" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D197" s="80" t="s">
+      <c r="D197" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E197" s="7" t="s">
+      <c r="E197" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="F197" s="80" t="s">
+      <c r="F197" s="3" t="s">
         <v>149</v>
       </c>
       <c r="G197" s="3" t="s">
@@ -11300,16 +11292,16 @@
         <v>1473</v>
       </c>
       <c r="J197" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K197" s="5"/>
       <c r="L197" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M197" s="7" t="s">
+      <c r="M197" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="N197" s="7" t="s">
+      <c r="N197" s="6" t="s">
         <v>265</v>
       </c>
       <c r="O197" s="2"/>
@@ -11323,17 +11315,17 @@
       <c r="A198" s="49">
         <v>11</v>
       </c>
-      <c r="B198" s="7" t="s">
+      <c r="B198" s="6" t="s">
         <v>266</v>
       </c>
       <c r="C198" s="80"/>
-      <c r="D198" s="80" t="s">
+      <c r="D198" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E198" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="F198" s="80" t="s">
+      <c r="E198" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="F198" s="3" t="s">
         <v>149</v>
       </c>
       <c r="G198" s="3" t="s">
@@ -11344,16 +11336,16 @@
         <v>1473</v>
       </c>
       <c r="J198" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K198" s="5"/>
       <c r="L198" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M198" s="7" t="s">
+      <c r="M198" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="N198" s="7" t="s">
+      <c r="N198" s="6" t="s">
         <v>265</v>
       </c>
       <c r="O198" s="2"/>
@@ -11367,19 +11359,19 @@
       <c r="A199" s="49">
         <v>11</v>
       </c>
-      <c r="B199" s="7" t="s">
+      <c r="B199" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="C199" s="80" t="s">
+      <c r="C199" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D199" s="80" t="s">
+      <c r="D199" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E199" s="7" t="s">
+      <c r="E199" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="F199" s="80" t="s">
+      <c r="F199" s="3" t="s">
         <v>107</v>
       </c>
       <c r="G199" s="3" t="s">
@@ -11393,13 +11385,13 @@
         <v>7.3</v>
       </c>
       <c r="K199" s="5"/>
-      <c r="L199" s="7" t="s">
+      <c r="L199" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M199" s="7" t="s">
+      <c r="M199" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="N199" s="7" t="s">
+      <c r="N199" s="6" t="s">
         <v>265</v>
       </c>
       <c r="O199" s="2"/>
@@ -11413,17 +11405,17 @@
       <c r="A200" s="49">
         <v>11</v>
       </c>
-      <c r="B200" s="7" t="s">
+      <c r="B200" s="6" t="s">
         <v>266</v>
       </c>
       <c r="C200" s="80"/>
-      <c r="D200" s="80" t="s">
+      <c r="D200" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E200" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="F200" s="80" t="s">
+      <c r="E200" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="F200" s="3" t="s">
         <v>107</v>
       </c>
       <c r="G200" s="3" t="s">
@@ -11437,13 +11429,13 @@
         <v>6.2</v>
       </c>
       <c r="K200" s="5"/>
-      <c r="L200" s="7" t="s">
+      <c r="L200" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M200" s="7" t="s">
+      <c r="M200" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="N200" s="7" t="s">
+      <c r="N200" s="6" t="s">
         <v>265</v>
       </c>
       <c r="O200" s="2"/>
@@ -11457,19 +11449,19 @@
       <c r="A201" s="49">
         <v>11</v>
       </c>
-      <c r="B201" s="7" t="s">
+      <c r="B201" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="C201" s="80" t="s">
+      <c r="C201" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D201" s="80" t="s">
+      <c r="D201" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E201" s="7" t="s">
+      <c r="E201" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="F201" s="80" t="s">
+      <c r="F201" s="3" t="s">
         <v>107</v>
       </c>
       <c r="G201" s="3" t="s">
@@ -11483,13 +11475,13 @@
         <v>9.1</v>
       </c>
       <c r="K201" s="5"/>
-      <c r="L201" s="7" t="s">
+      <c r="L201" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M201" s="7" t="s">
+      <c r="M201" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="N201" s="7" t="s">
+      <c r="N201" s="6" t="s">
         <v>265</v>
       </c>
       <c r="O201" s="2"/>
@@ -11503,19 +11495,19 @@
       <c r="A202" s="49">
         <v>11</v>
       </c>
-      <c r="B202" s="7" t="s">
+      <c r="B202" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="C202" s="80" t="s">
+      <c r="C202" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D202" s="80" t="s">
+      <c r="D202" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E202" s="7" t="s">
+      <c r="E202" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="F202" s="80" t="s">
+      <c r="F202" s="3" t="s">
         <v>107</v>
       </c>
       <c r="G202" s="3" t="s">
@@ -11529,13 +11521,13 @@
         <v>10.6</v>
       </c>
       <c r="K202" s="5"/>
-      <c r="L202" s="7" t="s">
+      <c r="L202" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M202" s="7" t="s">
+      <c r="M202" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="N202" s="7" t="s">
+      <c r="N202" s="6" t="s">
         <v>265</v>
       </c>
       <c r="O202" s="2"/>
@@ -11549,17 +11541,17 @@
       <c r="A203" s="49">
         <v>11</v>
       </c>
-      <c r="B203" s="7" t="s">
+      <c r="B203" s="6" t="s">
         <v>266</v>
       </c>
       <c r="C203" s="80"/>
-      <c r="D203" s="80" t="s">
+      <c r="D203" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E203" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="F203" s="80" t="s">
+      <c r="E203" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="F203" s="3" t="s">
         <v>107</v>
       </c>
       <c r="G203" s="3" t="s">
@@ -11573,13 +11565,13 @@
         <v>5.7</v>
       </c>
       <c r="K203" s="5"/>
-      <c r="L203" s="7" t="s">
+      <c r="L203" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M203" s="7" t="s">
+      <c r="M203" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="N203" s="7" t="s">
+      <c r="N203" s="6" t="s">
         <v>265</v>
       </c>
       <c r="O203" s="2"/>
@@ -11593,19 +11585,19 @@
       <c r="A204" s="49">
         <v>11</v>
       </c>
-      <c r="B204" s="7" t="s">
+      <c r="B204" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="C204" s="80" t="s">
+      <c r="C204" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D204" s="80" t="s">
+      <c r="D204" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E204" s="7" t="s">
+      <c r="E204" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="F204" s="80" t="s">
+      <c r="F204" s="3" t="s">
         <v>107</v>
       </c>
       <c r="G204" s="3" t="s">
@@ -11619,13 +11611,13 @@
         <v>0.8</v>
       </c>
       <c r="K204" s="5"/>
-      <c r="L204" s="7" t="s">
+      <c r="L204" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M204" s="7" t="s">
+      <c r="M204" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="N204" s="7" t="s">
+      <c r="N204" s="6" t="s">
         <v>265</v>
       </c>
       <c r="O204" s="2"/>
@@ -11639,17 +11631,17 @@
       <c r="A205" s="49">
         <v>11</v>
       </c>
-      <c r="B205" s="7" t="s">
+      <c r="B205" s="6" t="s">
         <v>266</v>
       </c>
       <c r="C205" s="80"/>
-      <c r="D205" s="80" t="s">
+      <c r="D205" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E205" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="F205" s="80" t="s">
+      <c r="E205" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="F205" s="3" t="s">
         <v>107</v>
       </c>
       <c r="G205" s="3" t="s">
@@ -11663,13 +11655,13 @@
         <v>8.3</v>
       </c>
       <c r="K205" s="5"/>
-      <c r="L205" s="7" t="s">
+      <c r="L205" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M205" s="7" t="s">
+      <c r="M205" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="N205" s="7" t="s">
+      <c r="N205" s="6" t="s">
         <v>265</v>
       </c>
       <c r="O205" s="2"/>
@@ -11683,19 +11675,19 @@
       <c r="A206" s="49">
         <v>12</v>
       </c>
-      <c r="B206" s="7" t="s">
+      <c r="B206" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C206" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D206" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="C206" s="80" t="s">
-        <v>65</v>
-      </c>
-      <c r="D206" s="80" t="s">
+      <c r="E206" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="E206" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="F206" s="80" t="s">
+      <c r="F206" s="3" t="s">
         <v>67</v>
       </c>
       <c r="G206" s="3" t="s">
@@ -11706,19 +11698,19 @@
         <v>298</v>
       </c>
       <c r="J206" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="K206" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="K206" s="5" t="s">
+      <c r="L206" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M206" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="N206" s="6" t="s">
         <v>283</v>
-      </c>
-      <c r="L206" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="M206" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="N206" s="7" t="s">
-        <v>284</v>
       </c>
       <c r="O206" s="2"/>
       <c r="P206" s="7"/>
@@ -11731,19 +11723,19 @@
       <c r="A207" s="49">
         <v>12</v>
       </c>
-      <c r="B207" s="7" t="s">
+      <c r="B207" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C207" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C207" s="80" t="s">
+      <c r="D207" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E207" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="D207" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E207" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="F207" s="80" t="s">
+      <c r="F207" s="3" t="s">
         <v>67</v>
       </c>
       <c r="G207" s="3" t="s">
@@ -11759,14 +11751,14 @@
       <c r="K207" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="L207" s="7" t="s">
+      <c r="L207" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M207" s="7" t="s">
+      <c r="M207" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="N207" s="7" t="s">
-        <v>284</v>
+      <c r="N207" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="O207" s="2"/>
       <c r="P207" s="7"/>
@@ -11779,19 +11771,19 @@
       <c r="A208" s="49">
         <v>12</v>
       </c>
-      <c r="B208" s="7" t="s">
+      <c r="B208" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C208" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D208" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E208" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="C208" s="80" t="s">
-        <v>286</v>
-      </c>
-      <c r="D208" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E208" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="F208" s="80" t="s">
+      <c r="F208" s="3" t="s">
         <v>67</v>
       </c>
       <c r="G208" s="3" t="s">
@@ -11802,19 +11794,19 @@
         <v>298</v>
       </c>
       <c r="J208" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K208" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L208" s="7" t="s">
+      <c r="L208" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M208" s="7" t="s">
+      <c r="M208" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="N208" s="7" t="s">
-        <v>284</v>
+      <c r="N208" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="O208" s="2"/>
       <c r="P208" s="7"/>
@@ -11827,20 +11819,20 @@
       <c r="A209" s="49">
         <v>12</v>
       </c>
-      <c r="B209" s="7" t="s">
+      <c r="B209" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D209" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="C209" s="80" t="s">
-        <v>65</v>
-      </c>
-      <c r="D209" s="80" t="s">
+      <c r="E209" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="E209" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="F209" s="80" t="s">
-        <v>291</v>
+      <c r="F209" s="3" t="s">
+        <v>290</v>
       </c>
       <c r="G209" s="3" t="s">
         <v>29</v>
@@ -11850,19 +11842,19 @@
         <v>298</v>
       </c>
       <c r="J209" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K209" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="L209" s="7" t="s">
+      <c r="L209" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M209" s="7" t="s">
+      <c r="M209" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="N209" s="7" t="s">
-        <v>284</v>
+      <c r="N209" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="O209" s="2"/>
       <c r="P209" s="7"/>
@@ -11875,20 +11867,20 @@
       <c r="A210" s="49">
         <v>12</v>
       </c>
-      <c r="B210" s="7" t="s">
+      <c r="B210" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C210" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C210" s="80" t="s">
+      <c r="D210" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E210" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="D210" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E210" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="F210" s="80" t="s">
-        <v>291</v>
+      <c r="F210" s="3" t="s">
+        <v>290</v>
       </c>
       <c r="G210" s="3" t="s">
         <v>29</v>
@@ -11898,19 +11890,19 @@
         <v>298</v>
       </c>
       <c r="J210" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="K210" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="K210" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="L210" s="7" t="s">
+      <c r="L210" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M210" s="7" t="s">
+      <c r="M210" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="N210" s="7" t="s">
-        <v>284</v>
+      <c r="N210" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="O210" s="2"/>
       <c r="P210" s="7"/>
@@ -11923,20 +11915,20 @@
       <c r="A211" s="49">
         <v>12</v>
       </c>
-      <c r="B211" s="7" t="s">
+      <c r="B211" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C211" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D211" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E211" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="C211" s="80" t="s">
-        <v>286</v>
-      </c>
-      <c r="D211" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E211" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="F211" s="80" t="s">
-        <v>291</v>
+      <c r="F211" s="3" t="s">
+        <v>290</v>
       </c>
       <c r="G211" s="3" t="s">
         <v>29</v>
@@ -11946,19 +11938,19 @@
         <v>298</v>
       </c>
       <c r="J211" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K211" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="L211" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M211" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="N211" s="6" t="s">
         <v>283</v>
-      </c>
-      <c r="L211" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="M211" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="N211" s="7" t="s">
-        <v>284</v>
       </c>
       <c r="O211" s="2"/>
       <c r="P211" s="7"/>
@@ -11971,19 +11963,19 @@
       <c r="A212" s="49">
         <v>12</v>
       </c>
-      <c r="B212" s="7" t="s">
+      <c r="B212" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C212" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D212" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="C212" s="80" t="s">
-        <v>65</v>
-      </c>
-      <c r="D212" s="80" t="s">
+      <c r="E212" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="E212" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="F212" s="80" t="s">
+      <c r="F212" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G212" s="3" t="s">
@@ -11999,14 +11991,14 @@
       <c r="K212" s="5">
         <v>0.4</v>
       </c>
-      <c r="L212" s="7" t="s">
+      <c r="L212" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M212" s="7" t="s">
+      <c r="M212" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="N212" s="7" t="s">
-        <v>284</v>
+      <c r="N212" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="O212" s="2"/>
       <c r="P212" s="7"/>
@@ -12019,19 +12011,19 @@
       <c r="A213" s="49">
         <v>12</v>
       </c>
-      <c r="B213" s="7" t="s">
+      <c r="B213" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C213" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C213" s="80" t="s">
+      <c r="D213" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E213" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="D213" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E213" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="F213" s="80" t="s">
+      <c r="F213" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G213" s="3" t="s">
@@ -12047,14 +12039,14 @@
       <c r="K213" s="5">
         <v>0.3</v>
       </c>
-      <c r="L213" s="7" t="s">
+      <c r="L213" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M213" s="7" t="s">
+      <c r="M213" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="N213" s="7" t="s">
-        <v>284</v>
+      <c r="N213" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="O213" s="2"/>
       <c r="P213" s="7"/>
@@ -12067,19 +12059,19 @@
       <c r="A214" s="49">
         <v>12</v>
       </c>
-      <c r="B214" s="7" t="s">
+      <c r="B214" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C214" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D214" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E214" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="C214" s="80" t="s">
-        <v>286</v>
-      </c>
-      <c r="D214" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E214" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="F214" s="80" t="s">
+      <c r="F214" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G214" s="3" t="s">
@@ -12095,14 +12087,14 @@
       <c r="K214" s="5">
         <v>0.1</v>
       </c>
-      <c r="L214" s="7" t="s">
+      <c r="L214" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M214" s="7" t="s">
+      <c r="M214" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="N214" s="7" t="s">
-        <v>284</v>
+      <c r="N214" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="O214" s="2"/>
       <c r="P214" s="7"/>
@@ -12115,20 +12107,20 @@
       <c r="A215" s="49">
         <v>12</v>
       </c>
-      <c r="B215" s="7" t="s">
+      <c r="B215" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C215" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D215" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="C215" s="80" t="s">
-        <v>65</v>
-      </c>
-      <c r="D215" s="80" t="s">
+      <c r="E215" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="E215" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="F215" s="80" t="s">
-        <v>296</v>
+      <c r="F215" s="3" t="s">
+        <v>295</v>
       </c>
       <c r="G215" s="3" t="s">
         <v>29</v>
@@ -12138,19 +12130,19 @@
         <v>298</v>
       </c>
       <c r="J215" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="K215" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="K215" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="L215" s="7" t="s">
+      <c r="L215" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M215" s="7" t="s">
+      <c r="M215" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="N215" s="7" t="s">
-        <v>284</v>
+      <c r="N215" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="O215" s="2"/>
       <c r="P215" s="7"/>
@@ -12163,20 +12155,20 @@
       <c r="A216" s="49">
         <v>12</v>
       </c>
-      <c r="B216" s="7" t="s">
+      <c r="B216" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C216" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C216" s="80" t="s">
+      <c r="D216" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E216" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="D216" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E216" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="F216" s="80" t="s">
-        <v>296</v>
+      <c r="F216" s="3" t="s">
+        <v>295</v>
       </c>
       <c r="G216" s="3" t="s">
         <v>29</v>
@@ -12186,19 +12178,19 @@
         <v>298</v>
       </c>
       <c r="J216" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="K216" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="K216" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="L216" s="7" t="s">
+      <c r="L216" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M216" s="7" t="s">
+      <c r="M216" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="N216" s="7" t="s">
-        <v>284</v>
+      <c r="N216" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="O216" s="2"/>
       <c r="P216" s="7"/>
@@ -12211,20 +12203,20 @@
       <c r="A217" s="49">
         <v>12</v>
       </c>
-      <c r="B217" s="7" t="s">
+      <c r="B217" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C217" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D217" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E217" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="C217" s="80" t="s">
-        <v>286</v>
-      </c>
-      <c r="D217" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E217" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="F217" s="80" t="s">
-        <v>296</v>
+      <c r="F217" s="3" t="s">
+        <v>295</v>
       </c>
       <c r="G217" s="3" t="s">
         <v>29</v>
@@ -12234,19 +12226,19 @@
         <v>298</v>
       </c>
       <c r="J217" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="K217" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="K217" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="L217" s="7" t="s">
+      <c r="L217" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M217" s="7" t="s">
+      <c r="M217" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="N217" s="7" t="s">
-        <v>284</v>
+      <c r="N217" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="O217" s="2"/>
       <c r="P217" s="7"/>
@@ -12259,19 +12251,19 @@
       <c r="A218" s="49">
         <v>12</v>
       </c>
-      <c r="B218" s="7" t="s">
+      <c r="B218" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C218" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D218" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="C218" s="80" t="s">
-        <v>65</v>
-      </c>
-      <c r="D218" s="80" t="s">
+      <c r="E218" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="E218" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="F218" s="80" t="s">
+      <c r="F218" s="3" t="s">
         <v>67</v>
       </c>
       <c r="G218" s="3" t="s">
@@ -12282,19 +12274,19 @@
         <v>773</v>
       </c>
       <c r="J218" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K218" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L218" s="7" t="s">
+      <c r="L218" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M218" s="7" t="s">
+      <c r="M218" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N218" s="7" t="s">
-        <v>284</v>
+      <c r="N218" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="O218" s="2"/>
       <c r="P218" s="7"/>
@@ -12307,19 +12299,19 @@
       <c r="A219" s="49">
         <v>12</v>
       </c>
-      <c r="B219" s="7" t="s">
+      <c r="B219" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C219" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C219" s="80" t="s">
+      <c r="D219" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E219" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="D219" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E219" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="F219" s="80" t="s">
+      <c r="F219" s="3" t="s">
         <v>67</v>
       </c>
       <c r="G219" s="3" t="s">
@@ -12330,19 +12322,19 @@
         <v>773</v>
       </c>
       <c r="J219" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K219" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="L219" s="7" t="s">
+      <c r="L219" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M219" s="7" t="s">
+      <c r="M219" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N219" s="7" t="s">
-        <v>284</v>
+      <c r="N219" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="O219" s="2"/>
       <c r="P219" s="7"/>
@@ -12355,19 +12347,19 @@
       <c r="A220" s="49">
         <v>12</v>
       </c>
-      <c r="B220" s="7" t="s">
+      <c r="B220" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C220" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D220" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E220" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="C220" s="80" t="s">
-        <v>286</v>
-      </c>
-      <c r="D220" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E220" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="F220" s="80" t="s">
+      <c r="F220" s="3" t="s">
         <v>67</v>
       </c>
       <c r="G220" s="3" t="s">
@@ -12378,19 +12370,19 @@
         <v>773</v>
       </c>
       <c r="J220" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="K220" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="K220" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="L220" s="7" t="s">
+      <c r="L220" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M220" s="7" t="s">
+      <c r="M220" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N220" s="7" t="s">
-        <v>284</v>
+      <c r="N220" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="O220" s="2"/>
       <c r="P220" s="7"/>
@@ -12403,19 +12395,19 @@
       <c r="A221" s="49">
         <v>12</v>
       </c>
-      <c r="B221" s="7" t="s">
+      <c r="B221" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C221" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D221" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="C221" s="80" t="s">
-        <v>65</v>
-      </c>
-      <c r="D221" s="80" t="s">
+      <c r="E221" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="E221" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="F221" s="80" t="s">
+      <c r="F221" s="3" t="s">
         <v>236</v>
       </c>
       <c r="G221" s="3" t="s">
@@ -12426,19 +12418,19 @@
         <v>773</v>
       </c>
       <c r="J221" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="K221" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="K221" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="L221" s="7" t="s">
+      <c r="L221" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M221" s="7" t="s">
+      <c r="M221" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N221" s="7" t="s">
-        <v>284</v>
+      <c r="N221" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="O221" s="2"/>
       <c r="P221" s="7"/>
@@ -12451,19 +12443,19 @@
       <c r="A222" s="49">
         <v>12</v>
       </c>
-      <c r="B222" s="7" t="s">
+      <c r="B222" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C222" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C222" s="80" t="s">
+      <c r="D222" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E222" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="D222" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E222" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="F222" s="80" t="s">
+      <c r="F222" s="3" t="s">
         <v>236</v>
       </c>
       <c r="G222" s="3" t="s">
@@ -12474,19 +12466,19 @@
         <v>773</v>
       </c>
       <c r="J222" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="K222" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="L222" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M222" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="N222" s="6" t="s">
         <v>283</v>
-      </c>
-      <c r="L222" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="M222" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="N222" s="7" t="s">
-        <v>284</v>
       </c>
       <c r="O222" s="2"/>
       <c r="P222" s="7"/>
@@ -12499,19 +12491,19 @@
       <c r="A223" s="49">
         <v>12</v>
       </c>
-      <c r="B223" s="7" t="s">
+      <c r="B223" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C223" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D223" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E223" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="C223" s="80" t="s">
-        <v>286</v>
-      </c>
-      <c r="D223" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E223" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="F223" s="80" t="s">
+      <c r="F223" s="3" t="s">
         <v>236</v>
       </c>
       <c r="G223" s="3" t="s">
@@ -12522,19 +12514,19 @@
         <v>773</v>
       </c>
       <c r="J223" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K223" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="L223" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="L223" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M223" s="7" t="s">
+      <c r="M223" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N223" s="7" t="s">
-        <v>284</v>
+      <c r="N223" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="O223" s="2"/>
       <c r="P223" s="7"/>
@@ -12547,19 +12539,19 @@
       <c r="A224" s="49">
         <v>12</v>
       </c>
-      <c r="B224" s="7" t="s">
+      <c r="B224" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C224" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D224" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="C224" s="80" t="s">
-        <v>65</v>
-      </c>
-      <c r="D224" s="80" t="s">
+      <c r="E224" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="E224" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="F224" s="80" t="s">
+      <c r="F224" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G224" s="3" t="s">
@@ -12575,14 +12567,14 @@
       <c r="K224" s="5">
         <v>0.6</v>
       </c>
-      <c r="L224" s="7" t="s">
+      <c r="L224" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M224" s="7" t="s">
+      <c r="M224" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N224" s="7" t="s">
-        <v>284</v>
+      <c r="N224" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="O224" s="2"/>
       <c r="P224" s="7"/>
@@ -12595,19 +12587,19 @@
       <c r="A225" s="49">
         <v>12</v>
       </c>
-      <c r="B225" s="7" t="s">
+      <c r="B225" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C225" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C225" s="80" t="s">
+      <c r="D225" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E225" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="D225" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E225" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="F225" s="80" t="s">
+      <c r="F225" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G225" s="3" t="s">
@@ -12623,14 +12615,14 @@
       <c r="K225" s="5">
         <v>0.8</v>
       </c>
-      <c r="L225" s="7" t="s">
+      <c r="L225" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M225" s="7" t="s">
+      <c r="M225" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N225" s="7" t="s">
-        <v>284</v>
+      <c r="N225" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="O225" s="2"/>
       <c r="P225" s="7"/>
@@ -12643,19 +12635,19 @@
       <c r="A226" s="49">
         <v>12</v>
       </c>
-      <c r="B226" s="7" t="s">
+      <c r="B226" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C226" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D226" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E226" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="C226" s="80" t="s">
-        <v>286</v>
-      </c>
-      <c r="D226" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E226" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="F226" s="80" t="s">
+      <c r="F226" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G226" s="3" t="s">
@@ -12671,14 +12663,14 @@
       <c r="K226" s="5">
         <v>2.6</v>
       </c>
-      <c r="L226" s="7" t="s">
+      <c r="L226" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M226" s="7" t="s">
+      <c r="M226" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="N226" s="7" t="s">
-        <v>284</v>
+      <c r="N226" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="O226" s="2"/>
       <c r="P226" s="7"/>
@@ -12691,19 +12683,19 @@
       <c r="A227" s="49">
         <v>12</v>
       </c>
-      <c r="B227" s="7" t="s">
+      <c r="B227" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C227" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D227" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="C227" s="80" t="s">
-        <v>65</v>
-      </c>
-      <c r="D227" s="80" t="s">
+      <c r="E227" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="E227" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="F227" s="80" t="s">
+      <c r="F227" s="3" t="s">
         <v>67</v>
       </c>
       <c r="G227" s="3" t="s">
@@ -12714,18 +12706,20 @@
         <v>973</v>
       </c>
       <c r="J227" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K227" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="L227" s="7" t="s">
+      <c r="L227" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M227" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="N227" s="7"/>
+      <c r="M227" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="N227" s="6" t="s">
+        <v>283</v>
+      </c>
       <c r="O227" s="2"/>
       <c r="P227" s="7"/>
       <c r="Q227" s="2"/>
@@ -12737,19 +12731,19 @@
       <c r="A228" s="49">
         <v>12</v>
       </c>
-      <c r="B228" s="7" t="s">
+      <c r="B228" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C228" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C228" s="80" t="s">
+      <c r="D228" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E228" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="D228" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E228" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="F228" s="80" t="s">
+      <c r="F228" s="3" t="s">
         <v>67</v>
       </c>
       <c r="G228" s="3" t="s">
@@ -12760,18 +12754,20 @@
         <v>973</v>
       </c>
       <c r="J228" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="K228" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="L228" s="7" t="s">
+      <c r="L228" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M228" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="N228" s="7"/>
+      <c r="M228" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="N228" s="6" t="s">
+        <v>283</v>
+      </c>
       <c r="O228" s="2"/>
       <c r="P228" s="7"/>
       <c r="Q228" s="2"/>
@@ -12783,19 +12779,19 @@
       <c r="A229" s="49">
         <v>12</v>
       </c>
-      <c r="B229" s="7" t="s">
+      <c r="B229" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C229" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D229" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E229" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="C229" s="80" t="s">
-        <v>286</v>
-      </c>
-      <c r="D229" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E229" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="F229" s="80" t="s">
+      <c r="F229" s="3" t="s">
         <v>67</v>
       </c>
       <c r="G229" s="3" t="s">
@@ -12806,18 +12802,20 @@
         <v>973</v>
       </c>
       <c r="J229" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="K229" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="L229" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M229" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="N229" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="L229" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="M229" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="N229" s="7"/>
       <c r="O229" s="2"/>
       <c r="P229" s="7"/>
       <c r="Q229" s="2"/>
@@ -12829,19 +12827,19 @@
       <c r="A230" s="49">
         <v>12</v>
       </c>
-      <c r="B230" s="7" t="s">
+      <c r="B230" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C230" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D230" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="C230" s="80" t="s">
-        <v>65</v>
-      </c>
-      <c r="D230" s="80" t="s">
+      <c r="E230" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="E230" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="F230" s="80" t="s">
+      <c r="F230" s="3" t="s">
         <v>236</v>
       </c>
       <c r="G230" s="3" t="s">
@@ -12852,18 +12850,20 @@
         <v>973</v>
       </c>
       <c r="J230" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="K230" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="L230" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="L230" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M230" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="N230" s="7"/>
+      <c r="M230" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="N230" s="6" t="s">
+        <v>283</v>
+      </c>
       <c r="O230" s="2"/>
       <c r="P230" s="7"/>
       <c r="Q230" s="2"/>
@@ -12875,19 +12875,19 @@
       <c r="A231" s="49">
         <v>12</v>
       </c>
-      <c r="B231" s="7" t="s">
+      <c r="B231" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C231" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C231" s="80" t="s">
+      <c r="D231" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E231" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="D231" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E231" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="F231" s="80" t="s">
+      <c r="F231" s="3" t="s">
         <v>236</v>
       </c>
       <c r="G231" s="3" t="s">
@@ -12898,18 +12898,20 @@
         <v>973</v>
       </c>
       <c r="J231" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K231" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="L231" s="7" t="s">
+      <c r="L231" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M231" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="N231" s="7"/>
+      <c r="M231" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="N231" s="6" t="s">
+        <v>283</v>
+      </c>
       <c r="O231" s="2"/>
       <c r="P231" s="7"/>
       <c r="Q231" s="2"/>
@@ -12921,19 +12923,19 @@
       <c r="A232" s="49">
         <v>12</v>
       </c>
-      <c r="B232" s="7" t="s">
+      <c r="B232" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C232" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D232" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E232" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="C232" s="80" t="s">
-        <v>286</v>
-      </c>
-      <c r="D232" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E232" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="F232" s="80" t="s">
+      <c r="F232" s="3" t="s">
         <v>236</v>
       </c>
       <c r="G232" s="3" t="s">
@@ -12944,18 +12946,20 @@
         <v>973</v>
       </c>
       <c r="J232" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K232" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="L232" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M232" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="N232" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="L232" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="M232" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="N232" s="7"/>
       <c r="O232" s="2"/>
       <c r="P232" s="7"/>
       <c r="Q232" s="2"/>
@@ -12967,19 +12971,19 @@
       <c r="A233" s="49">
         <v>12</v>
       </c>
-      <c r="B233" s="7" t="s">
+      <c r="B233" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C233" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D233" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="C233" s="80" t="s">
-        <v>65</v>
-      </c>
-      <c r="D233" s="80" t="s">
+      <c r="E233" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="E233" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="F233" s="80" t="s">
+      <c r="F233" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G233" s="3" t="s">
@@ -12995,13 +12999,15 @@
       <c r="K233" s="5">
         <v>1.6</v>
       </c>
-      <c r="L233" s="7" t="s">
+      <c r="L233" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M233" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="N233" s="7"/>
+      <c r="M233" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="N233" s="6" t="s">
+        <v>283</v>
+      </c>
       <c r="O233" s="2"/>
       <c r="P233" s="7"/>
       <c r="Q233" s="2"/>
@@ -13013,19 +13019,19 @@
       <c r="A234" s="49">
         <v>12</v>
       </c>
-      <c r="B234" s="7" t="s">
+      <c r="B234" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C234" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C234" s="80" t="s">
+      <c r="D234" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E234" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="D234" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E234" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="F234" s="80" t="s">
+      <c r="F234" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G234" s="3" t="s">
@@ -13041,13 +13047,15 @@
       <c r="K234" s="5">
         <v>0.5</v>
       </c>
-      <c r="L234" s="7" t="s">
+      <c r="L234" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M234" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="N234" s="7"/>
+      <c r="M234" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="N234" s="6" t="s">
+        <v>283</v>
+      </c>
       <c r="O234" s="2"/>
       <c r="P234" s="7"/>
       <c r="Q234" s="2"/>
@@ -13059,19 +13067,19 @@
       <c r="A235" s="49">
         <v>12</v>
       </c>
-      <c r="B235" s="7" t="s">
+      <c r="B235" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C235" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D235" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E235" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="C235" s="80" t="s">
-        <v>286</v>
-      </c>
-      <c r="D235" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E235" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="F235" s="80" t="s">
+      <c r="F235" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G235" s="3" t="s">
@@ -13087,13 +13095,15 @@
       <c r="K235" s="5">
         <v>1</v>
       </c>
-      <c r="L235" s="7" t="s">
+      <c r="L235" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M235" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="N235" s="7"/>
+      <c r="M235" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="N235" s="6" t="s">
+        <v>283</v>
+      </c>
       <c r="O235" s="2"/>
       <c r="P235" s="7"/>
       <c r="Q235" s="2"/>
@@ -13105,19 +13115,19 @@
       <c r="A236" s="49">
         <v>12</v>
       </c>
-      <c r="B236" s="7" t="s">
+      <c r="B236" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C236" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D236" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="C236" s="80" t="s">
-        <v>65</v>
-      </c>
-      <c r="D236" s="80" t="s">
+      <c r="E236" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="E236" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="F236" s="80" t="s">
+      <c r="F236" s="3" t="s">
         <v>67</v>
       </c>
       <c r="G236" s="3" t="s">
@@ -13128,14 +13138,20 @@
         <v>1173</v>
       </c>
       <c r="J236" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="K236" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="K236" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="L236" s="7"/>
-      <c r="M236" s="7"/>
-      <c r="N236" s="7"/>
+      <c r="L236" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M236" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="N236" s="6" t="s">
+        <v>283</v>
+      </c>
       <c r="O236" s="2"/>
       <c r="P236" s="7"/>
       <c r="Q236" s="2"/>
@@ -13147,19 +13163,19 @@
       <c r="A237" s="49">
         <v>12</v>
       </c>
-      <c r="B237" s="7" t="s">
+      <c r="B237" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C237" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C237" s="80" t="s">
+      <c r="D237" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E237" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="D237" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E237" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="F237" s="80" t="s">
+      <c r="F237" s="3" t="s">
         <v>67</v>
       </c>
       <c r="G237" s="3" t="s">
@@ -13170,14 +13186,20 @@
         <v>1173</v>
       </c>
       <c r="J237" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K237" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="L237" s="7"/>
-      <c r="M237" s="7"/>
-      <c r="N237" s="7"/>
+        <v>318</v>
+      </c>
+      <c r="L237" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M237" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="N237" s="6" t="s">
+        <v>283</v>
+      </c>
       <c r="O237" s="2"/>
       <c r="P237" s="7"/>
       <c r="Q237" s="2"/>
@@ -13189,19 +13211,19 @@
       <c r="A238" s="49">
         <v>12</v>
       </c>
-      <c r="B238" s="7" t="s">
+      <c r="B238" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C238" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D238" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E238" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="C238" s="80" t="s">
-        <v>286</v>
-      </c>
-      <c r="D238" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E238" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="F238" s="80" t="s">
+      <c r="F238" s="3" t="s">
         <v>67</v>
       </c>
       <c r="G238" s="3" t="s">
@@ -13212,14 +13234,20 @@
         <v>1173</v>
       </c>
       <c r="J238" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="K238" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="L238" s="7"/>
-      <c r="M238" s="7"/>
-      <c r="N238" s="7"/>
+        <v>293</v>
+      </c>
+      <c r="L238" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M238" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="N238" s="6" t="s">
+        <v>283</v>
+      </c>
       <c r="O238" s="2"/>
       <c r="P238" s="7"/>
       <c r="Q238" s="2"/>
@@ -13231,19 +13259,19 @@
       <c r="A239" s="49">
         <v>12</v>
       </c>
-      <c r="B239" s="7" t="s">
+      <c r="B239" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C239" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D239" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="C239" s="80" t="s">
-        <v>65</v>
-      </c>
-      <c r="D239" s="80" t="s">
+      <c r="E239" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="E239" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="F239" s="80" t="s">
+      <c r="F239" s="3" t="s">
         <v>236</v>
       </c>
       <c r="G239" s="3" t="s">
@@ -13254,14 +13282,20 @@
         <v>1173</v>
       </c>
       <c r="J239" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="K239" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="L239" s="7"/>
-      <c r="M239" s="7"/>
-      <c r="N239" s="7"/>
+        <v>318</v>
+      </c>
+      <c r="L239" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M239" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="N239" s="6" t="s">
+        <v>283</v>
+      </c>
       <c r="O239" s="2"/>
       <c r="P239" s="7"/>
       <c r="Q239" s="2"/>
@@ -13273,19 +13307,19 @@
       <c r="A240" s="49">
         <v>12</v>
       </c>
-      <c r="B240" s="7" t="s">
+      <c r="B240" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C240" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C240" s="80" t="s">
+      <c r="D240" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E240" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="D240" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E240" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="F240" s="80" t="s">
+      <c r="F240" s="3" t="s">
         <v>236</v>
       </c>
       <c r="G240" s="3" t="s">
@@ -13296,14 +13330,20 @@
         <v>1173</v>
       </c>
       <c r="J240" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K240" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="L240" s="7"/>
-      <c r="M240" s="7"/>
-      <c r="N240" s="7"/>
+        <v>318</v>
+      </c>
+      <c r="L240" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M240" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="N240" s="6" t="s">
+        <v>283</v>
+      </c>
       <c r="O240" s="2"/>
       <c r="P240" s="7"/>
       <c r="Q240" s="2"/>
@@ -13315,19 +13355,19 @@
       <c r="A241" s="49">
         <v>12</v>
       </c>
-      <c r="B241" s="7" t="s">
+      <c r="B241" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C241" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D241" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E241" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="C241" s="80" t="s">
-        <v>286</v>
-      </c>
-      <c r="D241" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E241" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="F241" s="80" t="s">
+      <c r="F241" s="3" t="s">
         <v>236</v>
       </c>
       <c r="G241" s="3" t="s">
@@ -13338,14 +13378,20 @@
         <v>1173</v>
       </c>
       <c r="J241" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K241" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="L241" s="7"/>
-      <c r="M241" s="7"/>
-      <c r="N241" s="7"/>
+        <v>293</v>
+      </c>
+      <c r="L241" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M241" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="N241" s="6" t="s">
+        <v>283</v>
+      </c>
       <c r="O241" s="2"/>
       <c r="P241" s="7"/>
       <c r="Q241" s="2"/>
@@ -13357,19 +13403,19 @@
       <c r="A242" s="49">
         <v>12</v>
       </c>
-      <c r="B242" s="7" t="s">
+      <c r="B242" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C242" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D242" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="C242" s="80" t="s">
-        <v>65</v>
-      </c>
-      <c r="D242" s="80" t="s">
+      <c r="E242" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="E242" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="F242" s="80" t="s">
+      <c r="F242" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G242" s="3" t="s">
@@ -13385,9 +13431,15 @@
       <c r="K242" s="5">
         <v>10.6</v>
       </c>
-      <c r="L242" s="7"/>
-      <c r="M242" s="7"/>
-      <c r="N242" s="7"/>
+      <c r="L242" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="M242" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="N242" s="6" t="s">
+        <v>283</v>
+      </c>
       <c r="O242" s="2"/>
       <c r="P242" s="7"/>
       <c r="Q242" s="2"/>
@@ -13399,19 +13451,19 @@
       <c r="A243" s="49">
         <v>12</v>
       </c>
-      <c r="B243" s="7" t="s">
+      <c r="B243" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C243" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C243" s="80" t="s">
+      <c r="D243" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E243" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="D243" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E243" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="F243" s="80" t="s">
+      <c r="F243" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G243" s="3" t="s">
@@ -13427,9 +13479,15 @@
       <c r="K243" s="5">
         <v>3.6</v>
       </c>
-      <c r="L243" s="7"/>
-      <c r="M243" s="7"/>
-      <c r="N243" s="7"/>
+      <c r="L243" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="M243" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="N243" s="6" t="s">
+        <v>283</v>
+      </c>
       <c r="O243" s="2"/>
       <c r="P243" s="7"/>
       <c r="Q243" s="2"/>
@@ -13441,19 +13499,19 @@
       <c r="A244" s="49">
         <v>12</v>
       </c>
-      <c r="B244" s="7" t="s">
+      <c r="B244" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C244" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D244" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E244" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="C244" s="80" t="s">
-        <v>286</v>
-      </c>
-      <c r="D244" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="E244" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="F244" s="80" t="s">
+      <c r="F244" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G244" s="3" t="s">
@@ -13469,9 +13527,15 @@
       <c r="K244" s="5">
         <v>2.2</v>
       </c>
-      <c r="L244" s="7"/>
-      <c r="M244" s="7"/>
-      <c r="N244" s="7"/>
+      <c r="L244" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="M244" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="N244" s="6" t="s">
+        <v>283</v>
+      </c>
       <c r="O244" s="2"/>
       <c r="P244" s="7"/>
       <c r="Q244" s="2"/>

</xml_diff>